<commit_message>
loop for was changed, outliers ere saved to vecor, added outliers style for excel wb
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -838,7 +838,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -856,8 +856,13 @@
       <sz val="11.0"/>
       <i val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -878,6 +883,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="D3D3D3"/>
+        <bgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="FF0000"/>
+        <bgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
@@ -962,7 +984,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -976,6 +998,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>

</xml_diff>

<commit_message>
outliers coloring not works
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -888,18 +888,18 @@
     </fill>
     <fill>
       <patternFill>
-        <fgColor rgb="FF0000"/>
+        <fgColor rgb="CD4F39"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill>
-        <fgColor rgb="FF0000"/>
+        <fgColor rgb="CD4F39"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0000"/>
+        <fgColor rgb="CD4F39"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
@@ -1316,10 +1316,10 @@
       <c r="AM3" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN3" t="s" s="8">
+      <c r="AN3" t="s">
         <v>37</v>
       </c>
-      <c r="AO3" s="8"/>
+      <c r="AO3"/>
       <c r="AP3" t="s">
         <v>162</v>
       </c>
@@ -1445,10 +1445,10 @@
       <c r="AM4" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN4" t="s" s="8">
+      <c r="AN4" t="s">
         <v>37</v>
       </c>
-      <c r="AO4" s="8"/>
+      <c r="AO4"/>
       <c r="AP4" t="s">
         <v>163</v>
       </c>
@@ -1574,10 +1574,10 @@
       <c r="AM5" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN5" t="s" s="8">
+      <c r="AN5" t="s">
         <v>37</v>
       </c>
-      <c r="AO5" s="8"/>
+      <c r="AO5"/>
       <c r="AP5" t="s">
         <v>164</v>
       </c>
@@ -1703,10 +1703,10 @@
       <c r="AM6" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN6" t="s" s="8">
+      <c r="AN6" t="s">
         <v>37</v>
       </c>
-      <c r="AO6" s="8"/>
+      <c r="AO6"/>
       <c r="AP6" t="s">
         <v>165</v>
       </c>
@@ -1832,10 +1832,10 @@
       <c r="AM7" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN7" t="s" s="8">
+      <c r="AN7" t="s">
         <v>37</v>
       </c>
-      <c r="AO7" s="8"/>
+      <c r="AO7"/>
       <c r="AP7" t="s">
         <v>166</v>
       </c>
@@ -1961,10 +1961,10 @@
       <c r="AM8" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN8" t="s" s="8">
+      <c r="AN8" t="s">
         <v>37</v>
       </c>
-      <c r="AO8" s="8"/>
+      <c r="AO8"/>
       <c r="AP8" t="s">
         <v>167</v>
       </c>
@@ -2090,10 +2090,10 @@
       <c r="AM9" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN9" t="s" s="8">
+      <c r="AN9" t="s">
         <v>37</v>
       </c>
-      <c r="AO9" s="8"/>
+      <c r="AO9"/>
       <c r="AP9" t="s">
         <v>168</v>
       </c>
@@ -2219,10 +2219,10 @@
       <c r="AM10" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN10" t="s" s="8">
+      <c r="AN10" t="s">
         <v>37</v>
       </c>
-      <c r="AO10" s="8"/>
+      <c r="AO10"/>
       <c r="AP10" t="s">
         <v>47</v>
       </c>
@@ -2348,10 +2348,10 @@
       <c r="AM11" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN11" t="s" s="8">
+      <c r="AN11" t="s">
         <v>37</v>
       </c>
-      <c r="AO11" s="8"/>
+      <c r="AO11"/>
       <c r="AP11" t="s">
         <v>169</v>
       </c>
@@ -2477,10 +2477,10 @@
       <c r="AM12" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN12" t="s" s="8">
+      <c r="AN12" t="s">
         <v>37</v>
       </c>
-      <c r="AO12" s="8"/>
+      <c r="AO12"/>
       <c r="AP12" t="s">
         <v>170</v>
       </c>
@@ -2606,10 +2606,10 @@
       <c r="AM13" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN13" t="s" s="8">
+      <c r="AN13" t="s">
         <v>37</v>
       </c>
-      <c r="AO13" s="8"/>
+      <c r="AO13"/>
       <c r="AP13" t="s">
         <v>171</v>
       </c>
@@ -2735,10 +2735,10 @@
       <c r="AM14" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN14" t="s" s="8">
+      <c r="AN14" t="s">
         <v>37</v>
       </c>
-      <c r="AO14" s="8"/>
+      <c r="AO14"/>
       <c r="AP14" t="s">
         <v>172</v>
       </c>
@@ -2864,10 +2864,10 @@
       <c r="AM15" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN15" t="s" s="8">
+      <c r="AN15" t="s">
         <v>37</v>
       </c>
-      <c r="AO15" s="8"/>
+      <c r="AO15"/>
       <c r="AP15" t="s">
         <v>173</v>
       </c>
@@ -2993,10 +2993,10 @@
       <c r="AM16" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN16" t="s" s="8">
+      <c r="AN16" t="s">
         <v>37</v>
       </c>
-      <c r="AO16" s="8"/>
+      <c r="AO16"/>
       <c r="AP16" t="s">
         <v>174</v>
       </c>
@@ -3122,10 +3122,10 @@
       <c r="AM17" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN17" t="s" s="8">
+      <c r="AN17" t="s">
         <v>37</v>
       </c>
-      <c r="AO17" s="8"/>
+      <c r="AO17"/>
       <c r="AP17" t="s">
         <v>175</v>
       </c>
@@ -3251,10 +3251,10 @@
       <c r="AM18" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN18" t="s" s="8">
+      <c r="AN18" t="s">
         <v>37</v>
       </c>
-      <c r="AO18" s="8"/>
+      <c r="AO18"/>
       <c r="AP18" t="s">
         <v>176</v>
       </c>
@@ -3380,10 +3380,10 @@
       <c r="AM19" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN19" t="s" s="8">
+      <c r="AN19" t="s">
         <v>37</v>
       </c>
-      <c r="AO19" s="8"/>
+      <c r="AO19"/>
       <c r="AP19" t="s">
         <v>177</v>
       </c>
@@ -3509,10 +3509,10 @@
       <c r="AM20" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN20" t="s" s="8">
+      <c r="AN20" t="s">
         <v>37</v>
       </c>
-      <c r="AO20" s="8"/>
+      <c r="AO20"/>
       <c r="AP20" t="s">
         <v>178</v>
       </c>
@@ -3638,10 +3638,10 @@
       <c r="AM21" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN21" t="s" s="8">
+      <c r="AN21" t="s">
         <v>37</v>
       </c>
-      <c r="AO21" s="8"/>
+      <c r="AO21"/>
       <c r="AP21" t="s">
         <v>179</v>
       </c>
@@ -3767,10 +3767,10 @@
       <c r="AM22" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN22" t="s" s="8">
+      <c r="AN22" t="s">
         <v>37</v>
       </c>
-      <c r="AO22" s="8"/>
+      <c r="AO22"/>
       <c r="AP22" t="s">
         <v>129</v>
       </c>
@@ -3896,10 +3896,10 @@
       <c r="AM23" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN23" t="s" s="8">
+      <c r="AN23" t="s">
         <v>37</v>
       </c>
-      <c r="AO23" s="8"/>
+      <c r="AO23"/>
       <c r="AP23" t="s">
         <v>180</v>
       </c>
@@ -4025,10 +4025,10 @@
       <c r="AM24" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN24" t="s" s="8">
+      <c r="AN24" t="s">
         <v>37</v>
       </c>
-      <c r="AO24" s="8"/>
+      <c r="AO24"/>
       <c r="AP24" t="s">
         <v>181</v>
       </c>
@@ -4154,10 +4154,10 @@
       <c r="AM25" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN25" t="s" s="8">
+      <c r="AN25" t="s">
         <v>37</v>
       </c>
-      <c r="AO25" s="8"/>
+      <c r="AO25"/>
       <c r="AP25" t="s">
         <v>182</v>
       </c>
@@ -4283,10 +4283,10 @@
       <c r="AM26" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN26" t="s" s="8">
+      <c r="AN26" t="s">
         <v>37</v>
       </c>
-      <c r="AO26" s="8"/>
+      <c r="AO26"/>
       <c r="AP26" t="s">
         <v>183</v>
       </c>
@@ -4379,8 +4379,8 @@
       <c r="AB27" t="n">
         <v>5.0</v>
       </c>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="8"/>
+      <c r="AC27"/>
+      <c r="AD27"/>
       <c r="AE27" t="n">
         <v>0.0</v>
       </c>
@@ -4408,10 +4408,10 @@
       <c r="AM27" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN27" t="s" s="8">
+      <c r="AN27" t="s">
         <v>37</v>
       </c>
-      <c r="AO27" s="8"/>
+      <c r="AO27"/>
       <c r="AP27" t="s">
         <v>64</v>
       </c>
@@ -4537,10 +4537,10 @@
       <c r="AM28" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN28" t="s" s="8">
+      <c r="AN28" t="s">
         <v>37</v>
       </c>
-      <c r="AO28" s="8"/>
+      <c r="AO28"/>
       <c r="AP28" t="s">
         <v>184</v>
       </c>
@@ -4624,7 +4624,7 @@
       <c r="Y29" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z29" s="8"/>
+      <c r="Z29"/>
       <c r="AA29" t="n">
         <v>3.0</v>
       </c>
@@ -4664,10 +4664,10 @@
       <c r="AM29" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN29" t="s" s="8">
+      <c r="AN29" t="s">
         <v>37</v>
       </c>
-      <c r="AO29" s="8"/>
+      <c r="AO29"/>
       <c r="AP29" t="s">
         <v>185</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="AA30" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB30" s="8"/>
+      <c r="AB30"/>
       <c r="AC30" t="n">
         <v>0.0</v>
       </c>
@@ -4791,10 +4791,10 @@
       <c r="AM30" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN30" t="s" s="8">
+      <c r="AN30" t="s">
         <v>37</v>
       </c>
-      <c r="AO30" s="8"/>
+      <c r="AO30"/>
       <c r="AP30" t="s">
         <v>186</v>
       </c>
@@ -4920,10 +4920,10 @@
       <c r="AM31" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN31" t="s" s="8">
+      <c r="AN31" t="s">
         <v>37</v>
       </c>
-      <c r="AO31" s="8"/>
+      <c r="AO31"/>
       <c r="AP31" t="s">
         <v>187</v>
       </c>
@@ -5049,10 +5049,10 @@
       <c r="AM32" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN32" t="s" s="8">
+      <c r="AN32" t="s">
         <v>37</v>
       </c>
-      <c r="AO32" s="8"/>
+      <c r="AO32"/>
       <c r="AP32" t="s">
         <v>188</v>
       </c>
@@ -5178,10 +5178,10 @@
       <c r="AM33" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN33" t="s" s="8">
+      <c r="AN33" t="s">
         <v>37</v>
       </c>
-      <c r="AO33" s="8"/>
+      <c r="AO33"/>
       <c r="AP33" t="s">
         <v>189</v>
       </c>
@@ -5268,11 +5268,11 @@
       <c r="Z34" t="n">
         <v>282.0</v>
       </c>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
-      <c r="AC34" s="8"/>
-      <c r="AD34" s="8"/>
-      <c r="AE34" s="8"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+      <c r="AE34"/>
       <c r="AF34" t="n">
         <v>1.0</v>
       </c>
@@ -5297,10 +5297,10 @@
       <c r="AM34" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN34" t="s" s="8">
+      <c r="AN34" t="s">
         <v>37</v>
       </c>
-      <c r="AO34" s="8"/>
+      <c r="AO34"/>
       <c r="AP34" t="s">
         <v>190</v>
       </c>
@@ -5426,10 +5426,10 @@
       <c r="AM35" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN35" t="s" s="8">
+      <c r="AN35" t="s">
         <v>37</v>
       </c>
-      <c r="AO35" s="8"/>
+      <c r="AO35"/>
       <c r="AP35" t="s">
         <v>191</v>
       </c>
@@ -5555,10 +5555,10 @@
       <c r="AM36" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN36" t="s" s="8">
+      <c r="AN36" t="s">
         <v>37</v>
       </c>
-      <c r="AO36" s="8"/>
+      <c r="AO36"/>
       <c r="AP36" t="s">
         <v>104</v>
       </c>
@@ -5684,10 +5684,10 @@
       <c r="AM37" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN37" t="s" s="8">
+      <c r="AN37" t="s">
         <v>37</v>
       </c>
-      <c r="AO37" s="8"/>
+      <c r="AO37"/>
       <c r="AP37" t="s">
         <v>192</v>
       </c>
@@ -5813,10 +5813,10 @@
       <c r="AM38" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN38" t="s" s="8">
+      <c r="AN38" t="s">
         <v>37</v>
       </c>
-      <c r="AO38" s="8"/>
+      <c r="AO38"/>
       <c r="AP38" t="s">
         <v>193</v>
       </c>
@@ -5909,8 +5909,8 @@
       <c r="AB39" t="n">
         <v>5.0</v>
       </c>
-      <c r="AC39" s="8"/>
-      <c r="AD39" s="8"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
       <c r="AE39" t="n">
         <v>1.0</v>
       </c>
@@ -5938,10 +5938,10 @@
       <c r="AM39" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN39" t="s" s="8">
+      <c r="AN39" t="s">
         <v>37</v>
       </c>
-      <c r="AO39" s="8"/>
+      <c r="AO39"/>
       <c r="AP39" t="s">
         <v>194</v>
       </c>
@@ -6067,10 +6067,10 @@
       <c r="AM40" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN40" t="s" s="8">
+      <c r="AN40" t="s">
         <v>37</v>
       </c>
-      <c r="AO40" s="8"/>
+      <c r="AO40"/>
       <c r="AP40" t="s">
         <v>195</v>
       </c>
@@ -6196,10 +6196,10 @@
       <c r="AM41" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN41" t="s" s="8">
+      <c r="AN41" t="s">
         <v>37</v>
       </c>
-      <c r="AO41" s="8"/>
+      <c r="AO41"/>
       <c r="AP41" t="s">
         <v>196</v>
       </c>
@@ -6325,10 +6325,10 @@
       <c r="AM42" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN42" t="s" s="8">
+      <c r="AN42" t="s">
         <v>37</v>
       </c>
-      <c r="AO42" s="8"/>
+      <c r="AO42"/>
       <c r="AP42" t="s">
         <v>197</v>
       </c>
@@ -6454,10 +6454,10 @@
       <c r="AM43" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN43" t="s" s="8">
+      <c r="AN43" t="s">
         <v>37</v>
       </c>
-      <c r="AO43" s="8"/>
+      <c r="AO43"/>
       <c r="AP43" t="s">
         <v>198</v>
       </c>
@@ -6583,10 +6583,10 @@
       <c r="AM44" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN44" t="s" s="8">
+      <c r="AN44" t="s">
         <v>37</v>
       </c>
-      <c r="AO44" s="8"/>
+      <c r="AO44"/>
       <c r="AP44" t="s">
         <v>199</v>
       </c>
@@ -6712,10 +6712,10 @@
       <c r="AM45" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN45" t="s" s="8">
+      <c r="AN45" t="s">
         <v>37</v>
       </c>
-      <c r="AO45" s="8"/>
+      <c r="AO45"/>
       <c r="AP45" t="s">
         <v>200</v>
       </c>
@@ -6841,10 +6841,10 @@
       <c r="AM46" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN46" t="s" s="8">
+      <c r="AN46" t="s">
         <v>37</v>
       </c>
-      <c r="AO46" s="8"/>
+      <c r="AO46"/>
       <c r="AP46" t="s">
         <v>201</v>
       </c>
@@ -6970,10 +6970,10 @@
       <c r="AM47" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN47" t="s" s="8">
+      <c r="AN47" t="s">
         <v>37</v>
       </c>
-      <c r="AO47" s="8"/>
+      <c r="AO47"/>
       <c r="AP47" t="s">
         <v>202</v>
       </c>
@@ -7099,10 +7099,10 @@
       <c r="AM48" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN48" t="s" s="8">
+      <c r="AN48" t="s">
         <v>37</v>
       </c>
-      <c r="AO48" s="8"/>
+      <c r="AO48"/>
       <c r="AP48" t="s">
         <v>84</v>
       </c>
@@ -7228,10 +7228,10 @@
       <c r="AM49" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN49" t="s" s="8">
+      <c r="AN49" t="s">
         <v>37</v>
       </c>
-      <c r="AO49" s="8"/>
+      <c r="AO49"/>
       <c r="AP49" t="s">
         <v>85</v>
       </c>
@@ -7357,10 +7357,10 @@
       <c r="AM50" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN50" t="s" s="8">
+      <c r="AN50" t="s">
         <v>37</v>
       </c>
-      <c r="AO50" s="8"/>
+      <c r="AO50"/>
       <c r="AP50" t="s">
         <v>203</v>
       </c>
@@ -7486,10 +7486,10 @@
       <c r="AM51" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN51" t="s" s="8">
+      <c r="AN51" t="s">
         <v>37</v>
       </c>
-      <c r="AO51" s="8"/>
+      <c r="AO51"/>
       <c r="AP51" t="s">
         <v>204</v>
       </c>
@@ -7615,10 +7615,10 @@
       <c r="AM52" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN52" t="s" s="8">
+      <c r="AN52" t="s">
         <v>37</v>
       </c>
-      <c r="AO52" s="8"/>
+      <c r="AO52"/>
       <c r="AP52" t="s">
         <v>205</v>
       </c>
@@ -7744,10 +7744,10 @@
       <c r="AM53" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN53" t="s" s="8">
+      <c r="AN53" t="s">
         <v>37</v>
       </c>
-      <c r="AO53" s="8"/>
+      <c r="AO53"/>
       <c r="AP53" t="s">
         <v>206</v>
       </c>
@@ -7882,7 +7882,7 @@
       <c r="AP54" t="s">
         <v>207</v>
       </c>
-      <c r="AQ54" t="s" s="8">
+      <c r="AQ54" t="s">
         <v>37</v>
       </c>
     </row>
@@ -7968,7 +7968,7 @@
       <c r="AA55" t="n">
         <v>2.0</v>
       </c>
-      <c r="AB55" s="8"/>
+      <c r="AB55"/>
       <c r="AC55" t="n">
         <v>1.0</v>
       </c>
@@ -8011,7 +8011,7 @@
       <c r="AP55" t="s">
         <v>193</v>
       </c>
-      <c r="AQ55" t="s" s="8">
+      <c r="AQ55" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8142,7 +8142,7 @@
       <c r="AP56" t="s">
         <v>208</v>
       </c>
-      <c r="AQ56" t="s" s="8">
+      <c r="AQ56" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8273,7 +8273,7 @@
       <c r="AP57" t="s">
         <v>209</v>
       </c>
-      <c r="AQ57" t="s" s="8">
+      <c r="AQ57" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8359,7 +8359,7 @@
       <c r="AA58" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB58" s="8"/>
+      <c r="AB58"/>
       <c r="AC58" t="n">
         <v>1.0</v>
       </c>
@@ -8402,7 +8402,7 @@
       <c r="AP58" t="s">
         <v>210</v>
       </c>
-      <c r="AQ58" t="s" s="8">
+      <c r="AQ58" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8488,7 +8488,7 @@
       <c r="AA59" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB59" s="8"/>
+      <c r="AB59"/>
       <c r="AC59" t="n">
         <v>1.0</v>
       </c>
@@ -8531,7 +8531,7 @@
       <c r="AP59" t="s">
         <v>211</v>
       </c>
-      <c r="AQ59" t="s" s="8">
+      <c r="AQ59" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8617,7 +8617,7 @@
       <c r="AA60" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB60" s="8"/>
+      <c r="AB60"/>
       <c r="AC60" t="n">
         <v>1.0</v>
       </c>
@@ -8660,7 +8660,7 @@
       <c r="AP60" t="s">
         <v>212</v>
       </c>
-      <c r="AQ60" t="s" s="8">
+      <c r="AQ60" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8791,7 +8791,7 @@
       <c r="AP61" t="s">
         <v>213</v>
       </c>
-      <c r="AQ61" t="s" s="8">
+      <c r="AQ61" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8877,7 +8877,7 @@
       <c r="AA62" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB62" s="8"/>
+      <c r="AB62"/>
       <c r="AC62" t="n">
         <v>1.0</v>
       </c>
@@ -8920,7 +8920,7 @@
       <c r="AP62" t="s">
         <v>214</v>
       </c>
-      <c r="AQ62" t="s" s="8">
+      <c r="AQ62" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9009,7 +9009,7 @@
       <c r="AB63" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC63" s="8"/>
+      <c r="AC63"/>
       <c r="AD63" t="n">
         <v>1.0</v>
       </c>
@@ -9049,7 +9049,7 @@
       <c r="AP63" t="s">
         <v>215</v>
       </c>
-      <c r="AQ63" t="s" s="8">
+      <c r="AQ63" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9135,7 +9135,7 @@
       <c r="AA64" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB64" s="8"/>
+      <c r="AB64"/>
       <c r="AC64" t="n">
         <v>1.0</v>
       </c>
@@ -9178,7 +9178,7 @@
       <c r="AP64" t="s">
         <v>216</v>
       </c>
-      <c r="AQ64" t="s" s="8">
+      <c r="AQ64" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9264,7 +9264,7 @@
       <c r="AA65" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB65" s="8"/>
+      <c r="AB65"/>
       <c r="AC65" t="n">
         <v>1.0</v>
       </c>
@@ -9307,7 +9307,7 @@
       <c r="AP65" t="s">
         <v>217</v>
       </c>
-      <c r="AQ65" t="s" s="8">
+      <c r="AQ65" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9393,8 +9393,8 @@
       <c r="AA66" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB66" s="8"/>
-      <c r="AC66" s="8"/>
+      <c r="AB66"/>
+      <c r="AC66"/>
       <c r="AD66" t="n">
         <v>1.0</v>
       </c>
@@ -9434,7 +9434,7 @@
       <c r="AP66" t="s">
         <v>218</v>
       </c>
-      <c r="AQ66" t="s" s="8">
+      <c r="AQ66" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9520,7 +9520,7 @@
       <c r="AA67" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB67" s="8"/>
+      <c r="AB67" s="12"/>
       <c r="AC67" t="n">
         <v>1.0</v>
       </c>
@@ -9563,7 +9563,7 @@
       <c r="AP67" t="s">
         <v>219</v>
       </c>
-      <c r="AQ67" t="s" s="8">
+      <c r="AQ67" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9649,7 +9649,7 @@
       <c r="AA68" t="n">
         <v>10.0</v>
       </c>
-      <c r="AB68" s="8"/>
+      <c r="AB68"/>
       <c r="AC68" t="n">
         <v>1.0</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="AP68" t="s">
         <v>220</v>
       </c>
-      <c r="AQ68" t="s" s="8">
+      <c r="AQ68" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9781,7 +9781,7 @@
       <c r="AB69" t="n">
         <v>21.0</v>
       </c>
-      <c r="AC69" s="8"/>
+      <c r="AC69"/>
       <c r="AD69" t="n">
         <v>1.0</v>
       </c>
@@ -9821,7 +9821,7 @@
       <c r="AP69" t="s">
         <v>221</v>
       </c>
-      <c r="AQ69" t="s" s="8">
+      <c r="AQ69" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9907,8 +9907,8 @@
       <c r="AA70" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB70" s="8"/>
-      <c r="AC70" s="8"/>
+      <c r="AB70"/>
+      <c r="AC70"/>
       <c r="AD70" t="n">
         <v>1.0</v>
       </c>
@@ -9948,7 +9948,7 @@
       <c r="AP70" t="s">
         <v>222</v>
       </c>
-      <c r="AQ70" t="s" s="8">
+      <c r="AQ70" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10034,11 +10034,11 @@
       <c r="AA71" t="n">
         <v>3.0</v>
       </c>
-      <c r="AB71" s="8"/>
+      <c r="AB71"/>
       <c r="AC71" t="n">
         <v>1.0</v>
       </c>
-      <c r="AD71" s="8"/>
+      <c r="AD71"/>
       <c r="AE71" t="n">
         <v>0.0</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="AP71" t="s">
         <v>223</v>
       </c>
-      <c r="AQ71" t="s" s="8">
+      <c r="AQ71" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10161,7 +10161,7 @@
       <c r="AA72" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB72" s="8"/>
+      <c r="AB72"/>
       <c r="AC72" t="n">
         <v>1.0</v>
       </c>
@@ -10204,7 +10204,7 @@
       <c r="AP72" t="s">
         <v>224</v>
       </c>
-      <c r="AQ72" t="s" s="8">
+      <c r="AQ72" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10293,7 +10293,7 @@
       <c r="AB73" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC73" s="8"/>
+      <c r="AC73"/>
       <c r="AD73" t="n">
         <v>1.0</v>
       </c>
@@ -10333,7 +10333,7 @@
       <c r="AP73" t="s">
         <v>225</v>
       </c>
-      <c r="AQ73" t="s" s="8">
+      <c r="AQ73" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10419,7 +10419,7 @@
       <c r="AA74" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB74" s="8"/>
+      <c r="AB74"/>
       <c r="AC74" t="n">
         <v>1.0</v>
       </c>
@@ -10462,7 +10462,7 @@
       <c r="AP74" t="s">
         <v>226</v>
       </c>
-      <c r="AQ74" t="s" s="8">
+      <c r="AQ74" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10551,7 +10551,7 @@
       <c r="AB75" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC75" s="8"/>
+      <c r="AC75"/>
       <c r="AD75" t="n">
         <v>1.0</v>
       </c>
@@ -10591,7 +10591,7 @@
       <c r="AP75" t="s">
         <v>227</v>
       </c>
-      <c r="AQ75" t="s" s="8">
+      <c r="AQ75" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10680,8 +10680,8 @@
       <c r="AB76" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC76" s="8"/>
-      <c r="AD76" s="8"/>
+      <c r="AC76"/>
+      <c r="AD76"/>
       <c r="AE76" t="n">
         <v>0.0</v>
       </c>
@@ -10718,7 +10718,7 @@
       <c r="AP76" t="s">
         <v>228</v>
       </c>
-      <c r="AQ76" t="s" s="8">
+      <c r="AQ76" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10804,7 +10804,7 @@
       <c r="AA77" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB77" s="8"/>
+      <c r="AB77"/>
       <c r="AC77" t="n">
         <v>2.0</v>
       </c>
@@ -10847,7 +10847,7 @@
       <c r="AP77" t="s">
         <v>229</v>
       </c>
-      <c r="AQ77" t="s" s="8">
+      <c r="AQ77" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10936,7 +10936,7 @@
       <c r="AB78" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC78" s="8"/>
+      <c r="AC78"/>
       <c r="AD78" t="n">
         <v>1.0</v>
       </c>
@@ -10976,7 +10976,7 @@
       <c r="AP78" t="s">
         <v>230</v>
       </c>
-      <c r="AQ78" t="s" s="8">
+      <c r="AQ78" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11062,7 +11062,7 @@
       <c r="AA79" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB79" s="8"/>
+      <c r="AB79"/>
       <c r="AC79" t="n">
         <v>1.0</v>
       </c>
@@ -11105,7 +11105,7 @@
       <c r="AP79" t="s">
         <v>188</v>
       </c>
-      <c r="AQ79" t="s" s="8">
+      <c r="AQ79" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11191,7 +11191,7 @@
       <c r="AA80" t="n">
         <v>13.0</v>
       </c>
-      <c r="AB80" s="8"/>
+      <c r="AB80"/>
       <c r="AC80" t="n">
         <v>1.0</v>
       </c>
@@ -11234,7 +11234,7 @@
       <c r="AP80" t="s">
         <v>231</v>
       </c>
-      <c r="AQ80" t="s" s="8">
+      <c r="AQ80" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11365,7 +11365,7 @@
       <c r="AP81" t="s">
         <v>232</v>
       </c>
-      <c r="AQ81" t="s" s="8">
+      <c r="AQ81" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11454,7 +11454,7 @@
       <c r="AB82" t="n">
         <v>13.0</v>
       </c>
-      <c r="AC82" s="8"/>
+      <c r="AC82"/>
       <c r="AD82" t="n">
         <v>1.0</v>
       </c>
@@ -11494,7 +11494,7 @@
       <c r="AP82" t="s">
         <v>233</v>
       </c>
-      <c r="AQ82" t="s" s="8">
+      <c r="AQ82" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11583,7 +11583,7 @@
       <c r="AB83" t="n">
         <v>8.0</v>
       </c>
-      <c r="AC83" s="8"/>
+      <c r="AC83"/>
       <c r="AD83" t="n">
         <v>1.0</v>
       </c>
@@ -11623,7 +11623,7 @@
       <c r="AP83" t="s">
         <v>234</v>
       </c>
-      <c r="AQ83" t="s" s="8">
+      <c r="AQ83" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11709,7 +11709,7 @@
       <c r="AA84" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB84" s="8"/>
+      <c r="AB84"/>
       <c r="AC84" t="n">
         <v>1.0</v>
       </c>
@@ -11752,7 +11752,7 @@
       <c r="AP84" t="s">
         <v>235</v>
       </c>
-      <c r="AQ84" t="s" s="8">
+      <c r="AQ84" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11838,7 +11838,7 @@
       <c r="AA85" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB85" s="8"/>
+      <c r="AB85"/>
       <c r="AC85" t="n">
         <v>1.0</v>
       </c>
@@ -11881,7 +11881,7 @@
       <c r="AP85" t="s">
         <v>236</v>
       </c>
-      <c r="AQ85" t="s" s="8">
+      <c r="AQ85" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11970,7 +11970,7 @@
       <c r="AB86" t="n">
         <v>7.0</v>
       </c>
-      <c r="AC86" s="8"/>
+      <c r="AC86"/>
       <c r="AD86" t="n">
         <v>1.0</v>
       </c>
@@ -12010,7 +12010,7 @@
       <c r="AP86" t="s">
         <v>237</v>
       </c>
-      <c r="AQ86" t="s" s="8">
+      <c r="AQ86" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12096,7 +12096,7 @@
       <c r="AA87" t="n">
         <v>10.0</v>
       </c>
-      <c r="AB87" s="8"/>
+      <c r="AB87" s="12"/>
       <c r="AC87" t="n">
         <v>1.0</v>
       </c>
@@ -12139,7 +12139,7 @@
       <c r="AP87" t="s">
         <v>238</v>
       </c>
-      <c r="AQ87" t="s" s="8">
+      <c r="AQ87" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12225,7 +12225,7 @@
       <c r="AA88" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB88" s="8"/>
+      <c r="AB88"/>
       <c r="AC88" t="n">
         <v>1.0</v>
       </c>
@@ -12268,7 +12268,7 @@
       <c r="AP88" t="s">
         <v>239</v>
       </c>
-      <c r="AQ88" t="s" s="8">
+      <c r="AQ88" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12348,7 +12348,7 @@
       <c r="Y89" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z89" s="8"/>
+      <c r="Z89"/>
       <c r="AA89" t="n">
         <v>34.0</v>
       </c>
@@ -12397,7 +12397,7 @@
       <c r="AP89" t="s">
         <v>240</v>
       </c>
-      <c r="AQ89" t="s" s="8">
+      <c r="AQ89" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12477,11 +12477,11 @@
       <c r="Y90" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z90" s="8"/>
+      <c r="Z90"/>
       <c r="AA90" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB90" s="8"/>
+      <c r="AB90"/>
       <c r="AC90" t="n">
         <v>1.0</v>
       </c>
@@ -12524,7 +12524,7 @@
       <c r="AP90" t="s">
         <v>185</v>
       </c>
-      <c r="AQ90" t="s" s="8">
+      <c r="AQ90" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12610,7 +12610,7 @@
       <c r="AA91" t="n">
         <v>8.0</v>
       </c>
-      <c r="AB91" s="8"/>
+      <c r="AB91"/>
       <c r="AC91" t="n">
         <v>1.0</v>
       </c>
@@ -12653,7 +12653,7 @@
       <c r="AP91" t="s">
         <v>241</v>
       </c>
-      <c r="AQ91" t="s" s="8">
+      <c r="AQ91" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12739,7 +12739,7 @@
       <c r="AA92" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB92" s="8"/>
+      <c r="AB92"/>
       <c r="AC92" t="n">
         <v>1.0</v>
       </c>
@@ -12782,7 +12782,7 @@
       <c r="AP92" t="s">
         <v>242</v>
       </c>
-      <c r="AQ92" t="s" s="8">
+      <c r="AQ92" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12871,7 +12871,7 @@
       <c r="AB93" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC93" s="8"/>
+      <c r="AC93"/>
       <c r="AD93" t="n">
         <v>2.0</v>
       </c>
@@ -12911,7 +12911,7 @@
       <c r="AP93" t="s">
         <v>150</v>
       </c>
-      <c r="AQ93" t="s" s="8">
+      <c r="AQ93" t="s">
         <v>37</v>
       </c>
     </row>
@@ -12997,7 +12997,7 @@
       <c r="AA94" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB94" s="8"/>
+      <c r="AB94"/>
       <c r="AC94" t="n">
         <v>1.0</v>
       </c>
@@ -13040,7 +13040,7 @@
       <c r="AP94" t="s">
         <v>243</v>
       </c>
-      <c r="AQ94" t="s" s="8">
+      <c r="AQ94" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13129,7 +13129,7 @@
       <c r="AB95" t="n">
         <v>14.0</v>
       </c>
-      <c r="AC95" s="8"/>
+      <c r="AC95"/>
       <c r="AD95" t="n">
         <v>1.0</v>
       </c>
@@ -13169,7 +13169,7 @@
       <c r="AP95" t="s">
         <v>244</v>
       </c>
-      <c r="AQ95" t="s" s="8">
+      <c r="AQ95" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13255,7 +13255,7 @@
       <c r="AA96" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB96" s="8"/>
+      <c r="AB96"/>
       <c r="AC96" t="n">
         <v>1.0</v>
       </c>
@@ -13298,7 +13298,7 @@
       <c r="AP96" t="s">
         <v>245</v>
       </c>
-      <c r="AQ96" t="s" s="8">
+      <c r="AQ96" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13381,8 +13381,8 @@
       <c r="Z97" t="n">
         <v>467.0</v>
       </c>
-      <c r="AA97" s="8"/>
-      <c r="AB97" s="8"/>
+      <c r="AA97"/>
+      <c r="AB97"/>
       <c r="AC97" t="n">
         <v>1.0</v>
       </c>
@@ -13425,7 +13425,7 @@
       <c r="AP97" t="s">
         <v>246</v>
       </c>
-      <c r="AQ97" t="s" s="8">
+      <c r="AQ97" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13511,8 +13511,8 @@
       <c r="AA98" t="n">
         <v>18.0</v>
       </c>
-      <c r="AB98" s="8"/>
-      <c r="AC98" s="8"/>
+      <c r="AB98"/>
+      <c r="AC98"/>
       <c r="AD98" t="n">
         <v>1.0</v>
       </c>
@@ -13552,7 +13552,7 @@
       <c r="AP98" t="s">
         <v>154</v>
       </c>
-      <c r="AQ98" t="s" s="8">
+      <c r="AQ98" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13638,7 +13638,7 @@
       <c r="AA99" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB99" s="8"/>
+      <c r="AB99"/>
       <c r="AC99" t="n">
         <v>1.0</v>
       </c>
@@ -13681,7 +13681,7 @@
       <c r="AP99" t="s">
         <v>247</v>
       </c>
-      <c r="AQ99" t="s" s="8">
+      <c r="AQ99" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13767,7 +13767,7 @@
       <c r="AA100" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB100" s="8"/>
+      <c r="AB100"/>
       <c r="AC100" t="n">
         <v>1.0</v>
       </c>
@@ -13810,7 +13810,7 @@
       <c r="AP100" t="s">
         <v>248</v>
       </c>
-      <c r="AQ100" t="s" s="8">
+      <c r="AQ100" t="s">
         <v>37</v>
       </c>
     </row>
@@ -13896,11 +13896,11 @@
       <c r="AA101" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB101" s="8"/>
+      <c r="AB101"/>
       <c r="AC101" t="n">
         <v>1.0</v>
       </c>
-      <c r="AD101" s="8"/>
+      <c r="AD101"/>
       <c r="AE101" t="n">
         <v>0.0</v>
       </c>
@@ -13937,7 +13937,7 @@
       <c r="AP101" t="s">
         <v>249</v>
       </c>
-      <c r="AQ101" t="s" s="8">
+      <c r="AQ101" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14023,7 +14023,7 @@
       <c r="AA102" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB102" s="8"/>
+      <c r="AB102"/>
       <c r="AC102" t="n">
         <v>1.0</v>
       </c>
@@ -14066,7 +14066,7 @@
       <c r="AP102" t="s">
         <v>250</v>
       </c>
-      <c r="AQ102" t="s" s="8">
+      <c r="AQ102" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14155,7 +14155,7 @@
       <c r="AB103" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC103" s="8"/>
+      <c r="AC103"/>
       <c r="AD103" t="n">
         <v>1.0</v>
       </c>
@@ -14195,7 +14195,7 @@
       <c r="AP103" t="s">
         <v>251</v>
       </c>
-      <c r="AQ103" t="s" s="8">
+      <c r="AQ103" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14281,7 +14281,7 @@
       <c r="AA104" t="n">
         <v>3.0</v>
       </c>
-      <c r="AB104" s="8"/>
+      <c r="AB104"/>
       <c r="AC104" t="n">
         <v>1.0</v>
       </c>
@@ -14324,7 +14324,7 @@
       <c r="AP104" t="s">
         <v>245</v>
       </c>
-      <c r="AQ104" t="s" s="8">
+      <c r="AQ104" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14413,7 +14413,7 @@
       <c r="AB105" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC105" s="8"/>
+      <c r="AC105"/>
       <c r="AD105" t="n">
         <v>1.0</v>
       </c>
@@ -14453,7 +14453,7 @@
       <c r="AP105" t="s">
         <v>252</v>
       </c>
-      <c r="AQ105" t="s" s="8">
+      <c r="AQ105" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14584,7 +14584,7 @@
       <c r="AP106" t="s">
         <v>253</v>
       </c>
-      <c r="AQ106" t="s" s="8">
+      <c r="AQ106" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14670,7 +14670,7 @@
       <c r="AA107" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB107" s="8"/>
+      <c r="AB107"/>
       <c r="AC107" t="n">
         <v>1.0</v>
       </c>
@@ -14701,7 +14701,7 @@
       <c r="AL107" t="n">
         <v>0.0</v>
       </c>
-      <c r="AM107" s="8"/>
+      <c r="AM107"/>
       <c r="AN107" t="s">
         <v>160</v>
       </c>
@@ -14711,7 +14711,7 @@
       <c r="AP107" t="s">
         <v>254</v>
       </c>
-      <c r="AQ107" t="s" s="8">
+      <c r="AQ107" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14797,7 +14797,7 @@
       <c r="AA108" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB108" s="8"/>
+      <c r="AB108"/>
       <c r="AC108" t="n">
         <v>1.0</v>
       </c>
@@ -14840,7 +14840,7 @@
       <c r="AP108" t="s">
         <v>255</v>
       </c>
-      <c r="AQ108" t="s" s="8">
+      <c r="AQ108" t="s">
         <v>37</v>
       </c>
     </row>
@@ -14929,7 +14929,7 @@
       <c r="AB109" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC109" s="8"/>
+      <c r="AC109"/>
       <c r="AD109" t="n">
         <v>1.0</v>
       </c>
@@ -14969,7 +14969,7 @@
       <c r="AP109" t="s">
         <v>256</v>
       </c>
-      <c r="AQ109" t="s" s="8">
+      <c r="AQ109" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15058,7 +15058,7 @@
       <c r="AB110" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC110" s="8"/>
+      <c r="AC110"/>
       <c r="AD110" t="n">
         <v>1.0</v>
       </c>
@@ -15098,7 +15098,7 @@
       <c r="AP110" t="s">
         <v>257</v>
       </c>
-      <c r="AQ110" t="s" s="8">
+      <c r="AQ110" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15184,7 +15184,7 @@
       <c r="AA111" t="n">
         <v>26.0</v>
       </c>
-      <c r="AB111" s="8"/>
+      <c r="AB111"/>
       <c r="AC111" t="n">
         <v>3.0</v>
       </c>
@@ -15227,7 +15227,7 @@
       <c r="AP111" t="s">
         <v>258</v>
       </c>
-      <c r="AQ111" t="s" s="8">
+      <c r="AQ111" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15358,7 +15358,7 @@
       <c r="AP112" t="s">
         <v>259</v>
       </c>
-      <c r="AQ112" t="s" s="8">
+      <c r="AQ112" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15444,7 +15444,7 @@
       <c r="AA113" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB113" s="8"/>
+      <c r="AB113"/>
       <c r="AC113" t="n">
         <v>1.0</v>
       </c>
@@ -15487,7 +15487,7 @@
       <c r="AP113" t="s">
         <v>260</v>
       </c>
-      <c r="AQ113" t="s" s="8">
+      <c r="AQ113" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15573,7 +15573,7 @@
       <c r="AA114" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB114" s="8"/>
+      <c r="AB114"/>
       <c r="AC114" t="n">
         <v>0.0</v>
       </c>
@@ -15616,7 +15616,7 @@
       <c r="AP114" t="s">
         <v>148</v>
       </c>
-      <c r="AQ114" t="s" s="8">
+      <c r="AQ114" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15747,7 +15747,7 @@
       <c r="AP115" t="s">
         <v>140</v>
       </c>
-      <c r="AQ115" t="s" s="8">
+      <c r="AQ115" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15833,7 +15833,7 @@
       <c r="AA116" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB116" s="8"/>
+      <c r="AB116"/>
       <c r="AC116" t="n">
         <v>1.0</v>
       </c>
@@ -15876,7 +15876,7 @@
       <c r="AP116" t="s">
         <v>261</v>
       </c>
-      <c r="AQ116" t="s" s="8">
+      <c r="AQ116" t="s">
         <v>37</v>
       </c>
     </row>
@@ -15962,7 +15962,7 @@
       <c r="AA117" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB117" s="8"/>
+      <c r="AB117"/>
       <c r="AC117" t="n">
         <v>1.0</v>
       </c>
@@ -16005,7 +16005,7 @@
       <c r="AP117" t="s">
         <v>262</v>
       </c>
-      <c r="AQ117" t="s" s="8">
+      <c r="AQ117" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16091,7 +16091,7 @@
       <c r="AA118" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB118" s="8"/>
+      <c r="AB118"/>
       <c r="AC118" t="n">
         <v>1.0</v>
       </c>
@@ -16134,7 +16134,7 @@
       <c r="AP118" t="s">
         <v>263</v>
       </c>
-      <c r="AQ118" t="s" s="8">
+      <c r="AQ118" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16265,7 +16265,7 @@
       <c r="AP119" t="s">
         <v>264</v>
       </c>
-      <c r="AQ119" t="s" s="8">
+      <c r="AQ119" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16351,7 +16351,7 @@
       <c r="AA120" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB120" s="8"/>
+      <c r="AB120"/>
       <c r="AC120" t="n">
         <v>1.0</v>
       </c>
@@ -16394,7 +16394,7 @@
       <c r="AP120" t="s">
         <v>265</v>
       </c>
-      <c r="AQ120" t="s" s="8">
+      <c r="AQ120" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16480,7 +16480,7 @@
       <c r="AA121" t="n">
         <v>9.0</v>
       </c>
-      <c r="AB121" s="8"/>
+      <c r="AB121"/>
       <c r="AC121" t="n">
         <v>1.0</v>
       </c>
@@ -16523,7 +16523,7 @@
       <c r="AP121" t="s">
         <v>97</v>
       </c>
-      <c r="AQ121" t="s" s="8">
+      <c r="AQ121" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16609,7 +16609,7 @@
       <c r="AA122" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB122" s="8"/>
+      <c r="AB122"/>
       <c r="AC122" t="n">
         <v>1.0</v>
       </c>
@@ -16652,7 +16652,7 @@
       <c r="AP122" t="s">
         <v>266</v>
       </c>
-      <c r="AQ122" t="s" s="8">
+      <c r="AQ122" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16738,7 +16738,7 @@
       <c r="AA123" t="n">
         <v>9.0</v>
       </c>
-      <c r="AB123" s="8"/>
+      <c r="AB123"/>
       <c r="AC123" t="n">
         <v>1.0</v>
       </c>
@@ -16781,7 +16781,7 @@
       <c r="AP123" t="s">
         <v>267</v>
       </c>
-      <c r="AQ123" t="s" s="8">
+      <c r="AQ123" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16867,7 +16867,7 @@
       <c r="AA124" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB124" s="8"/>
+      <c r="AB124"/>
       <c r="AC124" t="n">
         <v>2.0</v>
       </c>
@@ -16910,7 +16910,7 @@
       <c r="AP124" t="s">
         <v>153</v>
       </c>
-      <c r="AQ124" t="s" s="8">
+      <c r="AQ124" t="s">
         <v>37</v>
       </c>
     </row>
@@ -16996,7 +16996,7 @@
       <c r="AA125" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB125" s="8"/>
+      <c r="AB125"/>
       <c r="AC125" t="n">
         <v>1.0</v>
       </c>
@@ -17039,7 +17039,7 @@
       <c r="AP125" t="s">
         <v>268</v>
       </c>
-      <c r="AQ125" t="s" s="8">
+      <c r="AQ125" t="s">
         <v>37</v>
       </c>
     </row>
@@ -17161,10 +17161,10 @@
       <c r="AM126" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN126" t="s" s="8">
+      <c r="AN126" t="s">
         <v>37</v>
       </c>
-      <c r="AO126" s="8"/>
+      <c r="AO126"/>
       <c r="AP126" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
outliers coloring is not work, i don't known why
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -859,7 +859,7 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <b val="true"/>
+      <i val="true"/>
     </font>
   </fonts>
   <fills count="8">
@@ -888,18 +888,18 @@
     </fill>
     <fill>
       <patternFill>
-        <fgColor rgb="CD4F39"/>
+        <fgColor rgb="FF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill>
-        <fgColor rgb="CD4F39"/>
+        <fgColor rgb="FF0000"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="CD4F39"/>
+        <fgColor rgb="FF0000"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
@@ -1316,10 +1316,10 @@
       <c r="AM3" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO3"/>
+      <c r="AO3" s="8"/>
       <c r="AP3" t="s">
         <v>162</v>
       </c>
@@ -1445,10 +1445,10 @@
       <c r="AM4" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN4" t="s">
+      <c r="AN4" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO4"/>
+      <c r="AO4" s="8"/>
       <c r="AP4" t="s">
         <v>163</v>
       </c>
@@ -1574,10 +1574,10 @@
       <c r="AM5" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN5" t="s">
+      <c r="AN5" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO5"/>
+      <c r="AO5" s="8"/>
       <c r="AP5" t="s">
         <v>164</v>
       </c>
@@ -1703,10 +1703,10 @@
       <c r="AM6" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN6" t="s">
+      <c r="AN6" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO6"/>
+      <c r="AO6" s="8"/>
       <c r="AP6" t="s">
         <v>165</v>
       </c>
@@ -1832,10 +1832,10 @@
       <c r="AM7" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN7" t="s">
+      <c r="AN7" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO7"/>
+      <c r="AO7" s="8"/>
       <c r="AP7" t="s">
         <v>166</v>
       </c>
@@ -1961,10 +1961,10 @@
       <c r="AM8" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN8" t="s">
+      <c r="AN8" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO8"/>
+      <c r="AO8" s="8"/>
       <c r="AP8" t="s">
         <v>167</v>
       </c>
@@ -2090,10 +2090,10 @@
       <c r="AM9" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN9" t="s">
+      <c r="AN9" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO9"/>
+      <c r="AO9" s="8"/>
       <c r="AP9" t="s">
         <v>168</v>
       </c>
@@ -2219,10 +2219,10 @@
       <c r="AM10" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN10" t="s">
+      <c r="AN10" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO10"/>
+      <c r="AO10" s="8"/>
       <c r="AP10" t="s">
         <v>47</v>
       </c>
@@ -2348,10 +2348,10 @@
       <c r="AM11" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AN11" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO11"/>
+      <c r="AO11" s="8"/>
       <c r="AP11" t="s">
         <v>169</v>
       </c>
@@ -2477,10 +2477,10 @@
       <c r="AM12" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN12" t="s">
+      <c r="AN12" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO12"/>
+      <c r="AO12" s="8"/>
       <c r="AP12" t="s">
         <v>170</v>
       </c>
@@ -2606,10 +2606,10 @@
       <c r="AM13" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN13" t="s">
+      <c r="AN13" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO13"/>
+      <c r="AO13" s="8"/>
       <c r="AP13" t="s">
         <v>171</v>
       </c>
@@ -2735,10 +2735,10 @@
       <c r="AM14" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN14" t="s">
+      <c r="AN14" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO14"/>
+      <c r="AO14" s="8"/>
       <c r="AP14" t="s">
         <v>172</v>
       </c>
@@ -2864,10 +2864,10 @@
       <c r="AM15" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN15" t="s">
+      <c r="AN15" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO15"/>
+      <c r="AO15" s="8"/>
       <c r="AP15" t="s">
         <v>173</v>
       </c>
@@ -2993,10 +2993,10 @@
       <c r="AM16" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN16" t="s">
+      <c r="AN16" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO16"/>
+      <c r="AO16" s="8"/>
       <c r="AP16" t="s">
         <v>174</v>
       </c>
@@ -3122,10 +3122,10 @@
       <c r="AM17" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN17" t="s">
+      <c r="AN17" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO17"/>
+      <c r="AO17" s="8"/>
       <c r="AP17" t="s">
         <v>175</v>
       </c>
@@ -3251,10 +3251,10 @@
       <c r="AM18" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN18" t="s">
+      <c r="AN18" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO18"/>
+      <c r="AO18" s="8"/>
       <c r="AP18" t="s">
         <v>176</v>
       </c>
@@ -3380,10 +3380,10 @@
       <c r="AM19" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AN19" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO19"/>
+      <c r="AO19" s="8"/>
       <c r="AP19" t="s">
         <v>177</v>
       </c>
@@ -3509,10 +3509,10 @@
       <c r="AM20" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN20" t="s">
+      <c r="AN20" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO20"/>
+      <c r="AO20" s="8"/>
       <c r="AP20" t="s">
         <v>178</v>
       </c>
@@ -3638,10 +3638,10 @@
       <c r="AM21" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN21" t="s">
+      <c r="AN21" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO21"/>
+      <c r="AO21" s="8"/>
       <c r="AP21" t="s">
         <v>179</v>
       </c>
@@ -3767,10 +3767,10 @@
       <c r="AM22" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN22" t="s">
+      <c r="AN22" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO22"/>
+      <c r="AO22" s="8"/>
       <c r="AP22" t="s">
         <v>129</v>
       </c>
@@ -3896,10 +3896,10 @@
       <c r="AM23" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN23" t="s">
+      <c r="AN23" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO23"/>
+      <c r="AO23" s="8"/>
       <c r="AP23" t="s">
         <v>180</v>
       </c>
@@ -4025,10 +4025,10 @@
       <c r="AM24" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN24" t="s">
+      <c r="AN24" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO24"/>
+      <c r="AO24" s="8"/>
       <c r="AP24" t="s">
         <v>181</v>
       </c>
@@ -4154,10 +4154,10 @@
       <c r="AM25" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN25" t="s">
+      <c r="AN25" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO25"/>
+      <c r="AO25" s="8"/>
       <c r="AP25" t="s">
         <v>182</v>
       </c>
@@ -4283,10 +4283,10 @@
       <c r="AM26" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN26" t="s">
+      <c r="AN26" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO26"/>
+      <c r="AO26" s="8"/>
       <c r="AP26" t="s">
         <v>183</v>
       </c>
@@ -4379,8 +4379,8 @@
       <c r="AB27" t="n">
         <v>5.0</v>
       </c>
-      <c r="AC27"/>
-      <c r="AD27"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="8"/>
       <c r="AE27" t="n">
         <v>0.0</v>
       </c>
@@ -4408,10 +4408,10 @@
       <c r="AM27" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN27" t="s">
+      <c r="AN27" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO27"/>
+      <c r="AO27" s="8"/>
       <c r="AP27" t="s">
         <v>64</v>
       </c>
@@ -4537,10 +4537,10 @@
       <c r="AM28" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN28" t="s">
+      <c r="AN28" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO28"/>
+      <c r="AO28" s="8"/>
       <c r="AP28" t="s">
         <v>184</v>
       </c>
@@ -4624,7 +4624,7 @@
       <c r="Y29" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z29"/>
+      <c r="Z29" s="8"/>
       <c r="AA29" t="n">
         <v>3.0</v>
       </c>
@@ -4664,10 +4664,10 @@
       <c r="AM29" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN29" t="s">
+      <c r="AN29" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO29"/>
+      <c r="AO29" s="8"/>
       <c r="AP29" t="s">
         <v>185</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="AA30" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB30"/>
+      <c r="AB30" s="8"/>
       <c r="AC30" t="n">
         <v>0.0</v>
       </c>
@@ -4791,10 +4791,10 @@
       <c r="AM30" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN30" t="s">
+      <c r="AN30" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO30"/>
+      <c r="AO30" s="8"/>
       <c r="AP30" t="s">
         <v>186</v>
       </c>
@@ -4920,10 +4920,10 @@
       <c r="AM31" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN31" t="s">
+      <c r="AN31" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO31"/>
+      <c r="AO31" s="8"/>
       <c r="AP31" t="s">
         <v>187</v>
       </c>
@@ -5049,10 +5049,10 @@
       <c r="AM32" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN32" t="s">
+      <c r="AN32" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO32"/>
+      <c r="AO32" s="8"/>
       <c r="AP32" t="s">
         <v>188</v>
       </c>
@@ -5178,10 +5178,10 @@
       <c r="AM33" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN33" t="s">
+      <c r="AN33" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO33"/>
+      <c r="AO33" s="8"/>
       <c r="AP33" t="s">
         <v>189</v>
       </c>
@@ -5268,11 +5268,11 @@
       <c r="Z34" t="n">
         <v>282.0</v>
       </c>
-      <c r="AA34"/>
-      <c r="AB34"/>
-      <c r="AC34"/>
-      <c r="AD34"/>
-      <c r="AE34"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="8"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="8"/>
+      <c r="AE34" s="8"/>
       <c r="AF34" t="n">
         <v>1.0</v>
       </c>
@@ -5297,10 +5297,10 @@
       <c r="AM34" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN34" t="s">
+      <c r="AN34" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO34"/>
+      <c r="AO34" s="8"/>
       <c r="AP34" t="s">
         <v>190</v>
       </c>
@@ -5426,10 +5426,10 @@
       <c r="AM35" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN35" t="s">
+      <c r="AN35" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO35"/>
+      <c r="AO35" s="8"/>
       <c r="AP35" t="s">
         <v>191</v>
       </c>
@@ -5555,10 +5555,10 @@
       <c r="AM36" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN36" t="s">
+      <c r="AN36" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO36"/>
+      <c r="AO36" s="8"/>
       <c r="AP36" t="s">
         <v>104</v>
       </c>
@@ -5684,10 +5684,10 @@
       <c r="AM37" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN37" t="s">
+      <c r="AN37" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO37"/>
+      <c r="AO37" s="8"/>
       <c r="AP37" t="s">
         <v>192</v>
       </c>
@@ -5813,10 +5813,10 @@
       <c r="AM38" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN38" t="s">
+      <c r="AN38" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO38"/>
+      <c r="AO38" s="8"/>
       <c r="AP38" t="s">
         <v>193</v>
       </c>
@@ -5909,8 +5909,8 @@
       <c r="AB39" t="n">
         <v>5.0</v>
       </c>
-      <c r="AC39"/>
-      <c r="AD39"/>
+      <c r="AC39" s="8"/>
+      <c r="AD39" s="8"/>
       <c r="AE39" t="n">
         <v>1.0</v>
       </c>
@@ -5938,10 +5938,10 @@
       <c r="AM39" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN39" t="s">
+      <c r="AN39" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO39"/>
+      <c r="AO39" s="8"/>
       <c r="AP39" t="s">
         <v>194</v>
       </c>
@@ -6067,10 +6067,10 @@
       <c r="AM40" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN40" t="s">
+      <c r="AN40" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO40"/>
+      <c r="AO40" s="8"/>
       <c r="AP40" t="s">
         <v>195</v>
       </c>
@@ -6196,10 +6196,10 @@
       <c r="AM41" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN41" t="s">
+      <c r="AN41" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO41"/>
+      <c r="AO41" s="8"/>
       <c r="AP41" t="s">
         <v>196</v>
       </c>
@@ -6325,10 +6325,10 @@
       <c r="AM42" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN42" t="s">
+      <c r="AN42" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO42"/>
+      <c r="AO42" s="8"/>
       <c r="AP42" t="s">
         <v>197</v>
       </c>
@@ -6454,10 +6454,10 @@
       <c r="AM43" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN43" t="s">
+      <c r="AN43" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO43"/>
+      <c r="AO43" s="8"/>
       <c r="AP43" t="s">
         <v>198</v>
       </c>
@@ -6583,10 +6583,10 @@
       <c r="AM44" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN44" t="s">
+      <c r="AN44" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO44"/>
+      <c r="AO44" s="8"/>
       <c r="AP44" t="s">
         <v>199</v>
       </c>
@@ -6712,10 +6712,10 @@
       <c r="AM45" t="n">
         <v>3.0</v>
       </c>
-      <c r="AN45" t="s">
+      <c r="AN45" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO45"/>
+      <c r="AO45" s="8"/>
       <c r="AP45" t="s">
         <v>200</v>
       </c>
@@ -6841,10 +6841,10 @@
       <c r="AM46" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN46" t="s">
+      <c r="AN46" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO46"/>
+      <c r="AO46" s="8"/>
       <c r="AP46" t="s">
         <v>201</v>
       </c>
@@ -6970,10 +6970,10 @@
       <c r="AM47" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN47" t="s">
+      <c r="AN47" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO47"/>
+      <c r="AO47" s="8"/>
       <c r="AP47" t="s">
         <v>202</v>
       </c>
@@ -7099,10 +7099,10 @@
       <c r="AM48" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN48" t="s">
+      <c r="AN48" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO48"/>
+      <c r="AO48" s="8"/>
       <c r="AP48" t="s">
         <v>84</v>
       </c>
@@ -7228,10 +7228,10 @@
       <c r="AM49" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN49" t="s">
+      <c r="AN49" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO49"/>
+      <c r="AO49" s="8"/>
       <c r="AP49" t="s">
         <v>85</v>
       </c>
@@ -7357,10 +7357,10 @@
       <c r="AM50" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN50" t="s">
+      <c r="AN50" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO50"/>
+      <c r="AO50" s="8"/>
       <c r="AP50" t="s">
         <v>203</v>
       </c>
@@ -7486,10 +7486,10 @@
       <c r="AM51" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN51" t="s">
+      <c r="AN51" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO51"/>
+      <c r="AO51" s="8"/>
       <c r="AP51" t="s">
         <v>204</v>
       </c>
@@ -7615,10 +7615,10 @@
       <c r="AM52" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN52" t="s">
+      <c r="AN52" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO52"/>
+      <c r="AO52" s="8"/>
       <c r="AP52" t="s">
         <v>205</v>
       </c>
@@ -7744,10 +7744,10 @@
       <c r="AM53" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN53" t="s">
+      <c r="AN53" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO53"/>
+      <c r="AO53" s="8"/>
       <c r="AP53" t="s">
         <v>206</v>
       </c>
@@ -7882,7 +7882,7 @@
       <c r="AP54" t="s">
         <v>207</v>
       </c>
-      <c r="AQ54" t="s">
+      <c r="AQ54" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -7968,7 +7968,7 @@
       <c r="AA55" t="n">
         <v>2.0</v>
       </c>
-      <c r="AB55"/>
+      <c r="AB55" s="8"/>
       <c r="AC55" t="n">
         <v>1.0</v>
       </c>
@@ -8011,7 +8011,7 @@
       <c r="AP55" t="s">
         <v>193</v>
       </c>
-      <c r="AQ55" t="s">
+      <c r="AQ55" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8142,7 +8142,7 @@
       <c r="AP56" t="s">
         <v>208</v>
       </c>
-      <c r="AQ56" t="s">
+      <c r="AQ56" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8273,7 +8273,7 @@
       <c r="AP57" t="s">
         <v>209</v>
       </c>
-      <c r="AQ57" t="s">
+      <c r="AQ57" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8359,7 +8359,7 @@
       <c r="AA58" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB58"/>
+      <c r="AB58" s="8"/>
       <c r="AC58" t="n">
         <v>1.0</v>
       </c>
@@ -8402,7 +8402,7 @@
       <c r="AP58" t="s">
         <v>210</v>
       </c>
-      <c r="AQ58" t="s">
+      <c r="AQ58" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8488,7 +8488,7 @@
       <c r="AA59" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB59"/>
+      <c r="AB59" s="8"/>
       <c r="AC59" t="n">
         <v>1.0</v>
       </c>
@@ -8531,7 +8531,7 @@
       <c r="AP59" t="s">
         <v>211</v>
       </c>
-      <c r="AQ59" t="s">
+      <c r="AQ59" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8617,7 +8617,7 @@
       <c r="AA60" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB60"/>
+      <c r="AB60" s="8"/>
       <c r="AC60" t="n">
         <v>1.0</v>
       </c>
@@ -8660,7 +8660,7 @@
       <c r="AP60" t="s">
         <v>212</v>
       </c>
-      <c r="AQ60" t="s">
+      <c r="AQ60" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8791,7 +8791,7 @@
       <c r="AP61" t="s">
         <v>213</v>
       </c>
-      <c r="AQ61" t="s">
+      <c r="AQ61" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -8877,7 +8877,7 @@
       <c r="AA62" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB62"/>
+      <c r="AB62" s="8"/>
       <c r="AC62" t="n">
         <v>1.0</v>
       </c>
@@ -8920,7 +8920,7 @@
       <c r="AP62" t="s">
         <v>214</v>
       </c>
-      <c r="AQ62" t="s">
+      <c r="AQ62" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9009,7 +9009,7 @@
       <c r="AB63" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC63"/>
+      <c r="AC63" s="8"/>
       <c r="AD63" t="n">
         <v>1.0</v>
       </c>
@@ -9049,7 +9049,7 @@
       <c r="AP63" t="s">
         <v>215</v>
       </c>
-      <c r="AQ63" t="s">
+      <c r="AQ63" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9135,7 +9135,7 @@
       <c r="AA64" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB64"/>
+      <c r="AB64" s="8"/>
       <c r="AC64" t="n">
         <v>1.0</v>
       </c>
@@ -9178,7 +9178,7 @@
       <c r="AP64" t="s">
         <v>216</v>
       </c>
-      <c r="AQ64" t="s">
+      <c r="AQ64" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9264,7 +9264,7 @@
       <c r="AA65" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB65"/>
+      <c r="AB65" s="8"/>
       <c r="AC65" t="n">
         <v>1.0</v>
       </c>
@@ -9307,7 +9307,7 @@
       <c r="AP65" t="s">
         <v>217</v>
       </c>
-      <c r="AQ65" t="s">
+      <c r="AQ65" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9393,8 +9393,8 @@
       <c r="AA66" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB66"/>
-      <c r="AC66"/>
+      <c r="AB66" s="8"/>
+      <c r="AC66" s="8"/>
       <c r="AD66" t="n">
         <v>1.0</v>
       </c>
@@ -9434,7 +9434,7 @@
       <c r="AP66" t="s">
         <v>218</v>
       </c>
-      <c r="AQ66" t="s">
+      <c r="AQ66" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9520,7 +9520,7 @@
       <c r="AA67" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB67" s="12"/>
+      <c r="AB67" s="8"/>
       <c r="AC67" t="n">
         <v>1.0</v>
       </c>
@@ -9563,7 +9563,7 @@
       <c r="AP67" t="s">
         <v>219</v>
       </c>
-      <c r="AQ67" t="s">
+      <c r="AQ67" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9649,7 +9649,7 @@
       <c r="AA68" t="n">
         <v>10.0</v>
       </c>
-      <c r="AB68"/>
+      <c r="AB68" s="8"/>
       <c r="AC68" t="n">
         <v>1.0</v>
       </c>
@@ -9692,7 +9692,7 @@
       <c r="AP68" t="s">
         <v>220</v>
       </c>
-      <c r="AQ68" t="s">
+      <c r="AQ68" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9781,7 +9781,7 @@
       <c r="AB69" t="n">
         <v>21.0</v>
       </c>
-      <c r="AC69"/>
+      <c r="AC69" s="8"/>
       <c r="AD69" t="n">
         <v>1.0</v>
       </c>
@@ -9821,7 +9821,7 @@
       <c r="AP69" t="s">
         <v>221</v>
       </c>
-      <c r="AQ69" t="s">
+      <c r="AQ69" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -9907,8 +9907,8 @@
       <c r="AA70" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB70"/>
-      <c r="AC70"/>
+      <c r="AB70" s="8"/>
+      <c r="AC70" s="8"/>
       <c r="AD70" t="n">
         <v>1.0</v>
       </c>
@@ -9948,7 +9948,7 @@
       <c r="AP70" t="s">
         <v>222</v>
       </c>
-      <c r="AQ70" t="s">
+      <c r="AQ70" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10034,11 +10034,11 @@
       <c r="AA71" t="n">
         <v>3.0</v>
       </c>
-      <c r="AB71"/>
+      <c r="AB71" s="8"/>
       <c r="AC71" t="n">
         <v>1.0</v>
       </c>
-      <c r="AD71"/>
+      <c r="AD71" s="8"/>
       <c r="AE71" t="n">
         <v>0.0</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="AP71" t="s">
         <v>223</v>
       </c>
-      <c r="AQ71" t="s">
+      <c r="AQ71" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10161,7 +10161,7 @@
       <c r="AA72" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB72"/>
+      <c r="AB72" s="8"/>
       <c r="AC72" t="n">
         <v>1.0</v>
       </c>
@@ -10204,7 +10204,7 @@
       <c r="AP72" t="s">
         <v>224</v>
       </c>
-      <c r="AQ72" t="s">
+      <c r="AQ72" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10293,7 +10293,7 @@
       <c r="AB73" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC73"/>
+      <c r="AC73" s="8"/>
       <c r="AD73" t="n">
         <v>1.0</v>
       </c>
@@ -10333,7 +10333,7 @@
       <c r="AP73" t="s">
         <v>225</v>
       </c>
-      <c r="AQ73" t="s">
+      <c r="AQ73" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10419,7 +10419,7 @@
       <c r="AA74" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB74"/>
+      <c r="AB74" s="8"/>
       <c r="AC74" t="n">
         <v>1.0</v>
       </c>
@@ -10462,7 +10462,7 @@
       <c r="AP74" t="s">
         <v>226</v>
       </c>
-      <c r="AQ74" t="s">
+      <c r="AQ74" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10551,7 +10551,7 @@
       <c r="AB75" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC75"/>
+      <c r="AC75" s="8"/>
       <c r="AD75" t="n">
         <v>1.0</v>
       </c>
@@ -10591,7 +10591,7 @@
       <c r="AP75" t="s">
         <v>227</v>
       </c>
-      <c r="AQ75" t="s">
+      <c r="AQ75" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10680,8 +10680,8 @@
       <c r="AB76" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC76"/>
-      <c r="AD76"/>
+      <c r="AC76" s="8"/>
+      <c r="AD76" s="8"/>
       <c r="AE76" t="n">
         <v>0.0</v>
       </c>
@@ -10718,7 +10718,7 @@
       <c r="AP76" t="s">
         <v>228</v>
       </c>
-      <c r="AQ76" t="s">
+      <c r="AQ76" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10804,7 +10804,7 @@
       <c r="AA77" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB77"/>
+      <c r="AB77" s="8"/>
       <c r="AC77" t="n">
         <v>2.0</v>
       </c>
@@ -10847,7 +10847,7 @@
       <c r="AP77" t="s">
         <v>229</v>
       </c>
-      <c r="AQ77" t="s">
+      <c r="AQ77" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -10936,7 +10936,7 @@
       <c r="AB78" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC78"/>
+      <c r="AC78" s="8"/>
       <c r="AD78" t="n">
         <v>1.0</v>
       </c>
@@ -10976,7 +10976,7 @@
       <c r="AP78" t="s">
         <v>230</v>
       </c>
-      <c r="AQ78" t="s">
+      <c r="AQ78" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11062,7 +11062,7 @@
       <c r="AA79" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB79"/>
+      <c r="AB79" s="8"/>
       <c r="AC79" t="n">
         <v>1.0</v>
       </c>
@@ -11105,7 +11105,7 @@
       <c r="AP79" t="s">
         <v>188</v>
       </c>
-      <c r="AQ79" t="s">
+      <c r="AQ79" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11191,7 +11191,7 @@
       <c r="AA80" t="n">
         <v>13.0</v>
       </c>
-      <c r="AB80"/>
+      <c r="AB80" s="8"/>
       <c r="AC80" t="n">
         <v>1.0</v>
       </c>
@@ -11234,7 +11234,7 @@
       <c r="AP80" t="s">
         <v>231</v>
       </c>
-      <c r="AQ80" t="s">
+      <c r="AQ80" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11365,7 +11365,7 @@
       <c r="AP81" t="s">
         <v>232</v>
       </c>
-      <c r="AQ81" t="s">
+      <c r="AQ81" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11454,7 +11454,7 @@
       <c r="AB82" t="n">
         <v>13.0</v>
       </c>
-      <c r="AC82"/>
+      <c r="AC82" s="8"/>
       <c r="AD82" t="n">
         <v>1.0</v>
       </c>
@@ -11494,7 +11494,7 @@
       <c r="AP82" t="s">
         <v>233</v>
       </c>
-      <c r="AQ82" t="s">
+      <c r="AQ82" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11583,7 +11583,7 @@
       <c r="AB83" t="n">
         <v>8.0</v>
       </c>
-      <c r="AC83"/>
+      <c r="AC83" s="8"/>
       <c r="AD83" t="n">
         <v>1.0</v>
       </c>
@@ -11623,7 +11623,7 @@
       <c r="AP83" t="s">
         <v>234</v>
       </c>
-      <c r="AQ83" t="s">
+      <c r="AQ83" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11709,7 +11709,7 @@
       <c r="AA84" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB84"/>
+      <c r="AB84" s="8"/>
       <c r="AC84" t="n">
         <v>1.0</v>
       </c>
@@ -11752,7 +11752,7 @@
       <c r="AP84" t="s">
         <v>235</v>
       </c>
-      <c r="AQ84" t="s">
+      <c r="AQ84" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11838,7 +11838,7 @@
       <c r="AA85" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB85"/>
+      <c r="AB85" s="8"/>
       <c r="AC85" t="n">
         <v>1.0</v>
       </c>
@@ -11881,7 +11881,7 @@
       <c r="AP85" t="s">
         <v>236</v>
       </c>
-      <c r="AQ85" t="s">
+      <c r="AQ85" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -11970,7 +11970,7 @@
       <c r="AB86" t="n">
         <v>7.0</v>
       </c>
-      <c r="AC86"/>
+      <c r="AC86" s="8"/>
       <c r="AD86" t="n">
         <v>1.0</v>
       </c>
@@ -12010,7 +12010,7 @@
       <c r="AP86" t="s">
         <v>237</v>
       </c>
-      <c r="AQ86" t="s">
+      <c r="AQ86" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12096,7 +12096,7 @@
       <c r="AA87" t="n">
         <v>10.0</v>
       </c>
-      <c r="AB87" s="12"/>
+      <c r="AB87" s="8"/>
       <c r="AC87" t="n">
         <v>1.0</v>
       </c>
@@ -12139,7 +12139,7 @@
       <c r="AP87" t="s">
         <v>238</v>
       </c>
-      <c r="AQ87" t="s">
+      <c r="AQ87" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12225,7 +12225,7 @@
       <c r="AA88" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB88"/>
+      <c r="AB88" s="8"/>
       <c r="AC88" t="n">
         <v>1.0</v>
       </c>
@@ -12268,7 +12268,7 @@
       <c r="AP88" t="s">
         <v>239</v>
       </c>
-      <c r="AQ88" t="s">
+      <c r="AQ88" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12348,7 +12348,7 @@
       <c r="Y89" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z89"/>
+      <c r="Z89" s="8"/>
       <c r="AA89" t="n">
         <v>34.0</v>
       </c>
@@ -12397,7 +12397,7 @@
       <c r="AP89" t="s">
         <v>240</v>
       </c>
-      <c r="AQ89" t="s">
+      <c r="AQ89" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12477,11 +12477,11 @@
       <c r="Y90" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z90"/>
+      <c r="Z90" s="8"/>
       <c r="AA90" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB90"/>
+      <c r="AB90" s="8"/>
       <c r="AC90" t="n">
         <v>1.0</v>
       </c>
@@ -12524,7 +12524,7 @@
       <c r="AP90" t="s">
         <v>185</v>
       </c>
-      <c r="AQ90" t="s">
+      <c r="AQ90" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12610,7 +12610,7 @@
       <c r="AA91" t="n">
         <v>8.0</v>
       </c>
-      <c r="AB91"/>
+      <c r="AB91" s="8"/>
       <c r="AC91" t="n">
         <v>1.0</v>
       </c>
@@ -12653,7 +12653,7 @@
       <c r="AP91" t="s">
         <v>241</v>
       </c>
-      <c r="AQ91" t="s">
+      <c r="AQ91" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12739,7 +12739,7 @@
       <c r="AA92" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB92"/>
+      <c r="AB92" s="8"/>
       <c r="AC92" t="n">
         <v>1.0</v>
       </c>
@@ -12782,7 +12782,7 @@
       <c r="AP92" t="s">
         <v>242</v>
       </c>
-      <c r="AQ92" t="s">
+      <c r="AQ92" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12871,7 +12871,7 @@
       <c r="AB93" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC93"/>
+      <c r="AC93" s="8"/>
       <c r="AD93" t="n">
         <v>2.0</v>
       </c>
@@ -12911,7 +12911,7 @@
       <c r="AP93" t="s">
         <v>150</v>
       </c>
-      <c r="AQ93" t="s">
+      <c r="AQ93" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -12997,7 +12997,7 @@
       <c r="AA94" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB94"/>
+      <c r="AB94" s="8"/>
       <c r="AC94" t="n">
         <v>1.0</v>
       </c>
@@ -13040,7 +13040,7 @@
       <c r="AP94" t="s">
         <v>243</v>
       </c>
-      <c r="AQ94" t="s">
+      <c r="AQ94" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13129,7 +13129,7 @@
       <c r="AB95" t="n">
         <v>14.0</v>
       </c>
-      <c r="AC95"/>
+      <c r="AC95" s="8"/>
       <c r="AD95" t="n">
         <v>1.0</v>
       </c>
@@ -13169,7 +13169,7 @@
       <c r="AP95" t="s">
         <v>244</v>
       </c>
-      <c r="AQ95" t="s">
+      <c r="AQ95" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13255,7 +13255,7 @@
       <c r="AA96" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB96"/>
+      <c r="AB96" s="8"/>
       <c r="AC96" t="n">
         <v>1.0</v>
       </c>
@@ -13298,7 +13298,7 @@
       <c r="AP96" t="s">
         <v>245</v>
       </c>
-      <c r="AQ96" t="s">
+      <c r="AQ96" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13381,8 +13381,8 @@
       <c r="Z97" t="n">
         <v>467.0</v>
       </c>
-      <c r="AA97"/>
-      <c r="AB97"/>
+      <c r="AA97" s="8"/>
+      <c r="AB97" s="8"/>
       <c r="AC97" t="n">
         <v>1.0</v>
       </c>
@@ -13425,7 +13425,7 @@
       <c r="AP97" t="s">
         <v>246</v>
       </c>
-      <c r="AQ97" t="s">
+      <c r="AQ97" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13511,8 +13511,8 @@
       <c r="AA98" t="n">
         <v>18.0</v>
       </c>
-      <c r="AB98"/>
-      <c r="AC98"/>
+      <c r="AB98" s="8"/>
+      <c r="AC98" s="8"/>
       <c r="AD98" t="n">
         <v>1.0</v>
       </c>
@@ -13552,7 +13552,7 @@
       <c r="AP98" t="s">
         <v>154</v>
       </c>
-      <c r="AQ98" t="s">
+      <c r="AQ98" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13638,7 +13638,7 @@
       <c r="AA99" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB99"/>
+      <c r="AB99" s="8"/>
       <c r="AC99" t="n">
         <v>1.0</v>
       </c>
@@ -13681,7 +13681,7 @@
       <c r="AP99" t="s">
         <v>247</v>
       </c>
-      <c r="AQ99" t="s">
+      <c r="AQ99" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13767,7 +13767,7 @@
       <c r="AA100" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB100"/>
+      <c r="AB100" s="8"/>
       <c r="AC100" t="n">
         <v>1.0</v>
       </c>
@@ -13810,7 +13810,7 @@
       <c r="AP100" t="s">
         <v>248</v>
       </c>
-      <c r="AQ100" t="s">
+      <c r="AQ100" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -13896,11 +13896,11 @@
       <c r="AA101" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB101"/>
+      <c r="AB101" s="8"/>
       <c r="AC101" t="n">
         <v>1.0</v>
       </c>
-      <c r="AD101"/>
+      <c r="AD101" s="8"/>
       <c r="AE101" t="n">
         <v>0.0</v>
       </c>
@@ -13937,7 +13937,7 @@
       <c r="AP101" t="s">
         <v>249</v>
       </c>
-      <c r="AQ101" t="s">
+      <c r="AQ101" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14023,7 +14023,7 @@
       <c r="AA102" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB102"/>
+      <c r="AB102" s="8"/>
       <c r="AC102" t="n">
         <v>1.0</v>
       </c>
@@ -14066,7 +14066,7 @@
       <c r="AP102" t="s">
         <v>250</v>
       </c>
-      <c r="AQ102" t="s">
+      <c r="AQ102" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14155,7 +14155,7 @@
       <c r="AB103" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC103"/>
+      <c r="AC103" s="8"/>
       <c r="AD103" t="n">
         <v>1.0</v>
       </c>
@@ -14195,7 +14195,7 @@
       <c r="AP103" t="s">
         <v>251</v>
       </c>
-      <c r="AQ103" t="s">
+      <c r="AQ103" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14281,7 +14281,7 @@
       <c r="AA104" t="n">
         <v>3.0</v>
       </c>
-      <c r="AB104"/>
+      <c r="AB104" s="8"/>
       <c r="AC104" t="n">
         <v>1.0</v>
       </c>
@@ -14324,7 +14324,7 @@
       <c r="AP104" t="s">
         <v>245</v>
       </c>
-      <c r="AQ104" t="s">
+      <c r="AQ104" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14413,7 +14413,7 @@
       <c r="AB105" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC105"/>
+      <c r="AC105" s="8"/>
       <c r="AD105" t="n">
         <v>1.0</v>
       </c>
@@ -14453,7 +14453,7 @@
       <c r="AP105" t="s">
         <v>252</v>
       </c>
-      <c r="AQ105" t="s">
+      <c r="AQ105" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14584,7 +14584,7 @@
       <c r="AP106" t="s">
         <v>253</v>
       </c>
-      <c r="AQ106" t="s">
+      <c r="AQ106" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14670,7 +14670,7 @@
       <c r="AA107" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB107"/>
+      <c r="AB107" s="8"/>
       <c r="AC107" t="n">
         <v>1.0</v>
       </c>
@@ -14701,7 +14701,7 @@
       <c r="AL107" t="n">
         <v>0.0</v>
       </c>
-      <c r="AM107"/>
+      <c r="AM107" s="8"/>
       <c r="AN107" t="s">
         <v>160</v>
       </c>
@@ -14711,7 +14711,7 @@
       <c r="AP107" t="s">
         <v>254</v>
       </c>
-      <c r="AQ107" t="s">
+      <c r="AQ107" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14797,7 +14797,7 @@
       <c r="AA108" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB108"/>
+      <c r="AB108" s="8"/>
       <c r="AC108" t="n">
         <v>1.0</v>
       </c>
@@ -14840,7 +14840,7 @@
       <c r="AP108" t="s">
         <v>255</v>
       </c>
-      <c r="AQ108" t="s">
+      <c r="AQ108" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -14929,7 +14929,7 @@
       <c r="AB109" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC109"/>
+      <c r="AC109" s="8"/>
       <c r="AD109" t="n">
         <v>1.0</v>
       </c>
@@ -14969,7 +14969,7 @@
       <c r="AP109" t="s">
         <v>256</v>
       </c>
-      <c r="AQ109" t="s">
+      <c r="AQ109" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15058,7 +15058,7 @@
       <c r="AB110" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC110"/>
+      <c r="AC110" s="8"/>
       <c r="AD110" t="n">
         <v>1.0</v>
       </c>
@@ -15098,7 +15098,7 @@
       <c r="AP110" t="s">
         <v>257</v>
       </c>
-      <c r="AQ110" t="s">
+      <c r="AQ110" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15184,7 +15184,7 @@
       <c r="AA111" t="n">
         <v>26.0</v>
       </c>
-      <c r="AB111"/>
+      <c r="AB111" s="8"/>
       <c r="AC111" t="n">
         <v>3.0</v>
       </c>
@@ -15227,7 +15227,7 @@
       <c r="AP111" t="s">
         <v>258</v>
       </c>
-      <c r="AQ111" t="s">
+      <c r="AQ111" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15358,7 +15358,7 @@
       <c r="AP112" t="s">
         <v>259</v>
       </c>
-      <c r="AQ112" t="s">
+      <c r="AQ112" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15444,7 +15444,7 @@
       <c r="AA113" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB113"/>
+      <c r="AB113" s="8"/>
       <c r="AC113" t="n">
         <v>1.0</v>
       </c>
@@ -15487,7 +15487,7 @@
       <c r="AP113" t="s">
         <v>260</v>
       </c>
-      <c r="AQ113" t="s">
+      <c r="AQ113" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15573,7 +15573,7 @@
       <c r="AA114" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB114"/>
+      <c r="AB114" s="8"/>
       <c r="AC114" t="n">
         <v>0.0</v>
       </c>
@@ -15616,7 +15616,7 @@
       <c r="AP114" t="s">
         <v>148</v>
       </c>
-      <c r="AQ114" t="s">
+      <c r="AQ114" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15747,7 +15747,7 @@
       <c r="AP115" t="s">
         <v>140</v>
       </c>
-      <c r="AQ115" t="s">
+      <c r="AQ115" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15833,7 +15833,7 @@
       <c r="AA116" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB116"/>
+      <c r="AB116" s="8"/>
       <c r="AC116" t="n">
         <v>1.0</v>
       </c>
@@ -15876,7 +15876,7 @@
       <c r="AP116" t="s">
         <v>261</v>
       </c>
-      <c r="AQ116" t="s">
+      <c r="AQ116" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -15962,7 +15962,7 @@
       <c r="AA117" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB117"/>
+      <c r="AB117" s="8"/>
       <c r="AC117" t="n">
         <v>1.0</v>
       </c>
@@ -16005,7 +16005,7 @@
       <c r="AP117" t="s">
         <v>262</v>
       </c>
-      <c r="AQ117" t="s">
+      <c r="AQ117" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16091,7 +16091,7 @@
       <c r="AA118" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB118"/>
+      <c r="AB118" s="8"/>
       <c r="AC118" t="n">
         <v>1.0</v>
       </c>
@@ -16134,7 +16134,7 @@
       <c r="AP118" t="s">
         <v>263</v>
       </c>
-      <c r="AQ118" t="s">
+      <c r="AQ118" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16265,7 +16265,7 @@
       <c r="AP119" t="s">
         <v>264</v>
       </c>
-      <c r="AQ119" t="s">
+      <c r="AQ119" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16351,7 +16351,7 @@
       <c r="AA120" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB120"/>
+      <c r="AB120" s="8"/>
       <c r="AC120" t="n">
         <v>1.0</v>
       </c>
@@ -16394,7 +16394,7 @@
       <c r="AP120" t="s">
         <v>265</v>
       </c>
-      <c r="AQ120" t="s">
+      <c r="AQ120" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16480,7 +16480,7 @@
       <c r="AA121" t="n">
         <v>9.0</v>
       </c>
-      <c r="AB121"/>
+      <c r="AB121" s="8"/>
       <c r="AC121" t="n">
         <v>1.0</v>
       </c>
@@ -16523,7 +16523,7 @@
       <c r="AP121" t="s">
         <v>97</v>
       </c>
-      <c r="AQ121" t="s">
+      <c r="AQ121" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16609,7 +16609,7 @@
       <c r="AA122" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB122"/>
+      <c r="AB122" s="8"/>
       <c r="AC122" t="n">
         <v>1.0</v>
       </c>
@@ -16652,7 +16652,7 @@
       <c r="AP122" t="s">
         <v>266</v>
       </c>
-      <c r="AQ122" t="s">
+      <c r="AQ122" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16738,7 +16738,7 @@
       <c r="AA123" t="n">
         <v>9.0</v>
       </c>
-      <c r="AB123"/>
+      <c r="AB123" s="8"/>
       <c r="AC123" t="n">
         <v>1.0</v>
       </c>
@@ -16781,7 +16781,7 @@
       <c r="AP123" t="s">
         <v>267</v>
       </c>
-      <c r="AQ123" t="s">
+      <c r="AQ123" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16867,7 +16867,7 @@
       <c r="AA124" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB124"/>
+      <c r="AB124" s="8"/>
       <c r="AC124" t="n">
         <v>2.0</v>
       </c>
@@ -16910,7 +16910,7 @@
       <c r="AP124" t="s">
         <v>153</v>
       </c>
-      <c r="AQ124" t="s">
+      <c r="AQ124" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -16996,7 +16996,7 @@
       <c r="AA125" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB125"/>
+      <c r="AB125" s="8"/>
       <c r="AC125" t="n">
         <v>1.0</v>
       </c>
@@ -17039,7 +17039,7 @@
       <c r="AP125" t="s">
         <v>268</v>
       </c>
-      <c r="AQ125" t="s">
+      <c r="AQ125" t="s" s="8">
         <v>37</v>
       </c>
     </row>
@@ -17161,10 +17161,10 @@
       <c r="AM126" t="n">
         <v>1.0</v>
       </c>
-      <c r="AN126" t="s">
+      <c r="AN126" t="s" s="8">
         <v>37</v>
       </c>
-      <c r="AO126"/>
+      <c r="AO126" s="8"/>
       <c r="AP126" t="s">
         <v>269</v>
       </c>

</xml_diff>

<commit_message>
Hey! It's working. Outliers are colored
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -1403,7 +1403,7 @@
       <c r="Y4" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="Z4" t="n" s="12">
         <v>434.0</v>
       </c>
       <c r="AA4" t="n">
@@ -1592,7 +1592,7 @@
       <c r="B6" t="n">
         <v>1.0</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="n" s="12">
         <v>37.0</v>
       </c>
       <c r="D6" t="n">
@@ -1661,7 +1661,7 @@
       <c r="Y6" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="Z6" t="n" s="12">
         <v>410.0</v>
       </c>
       <c r="AA6" t="n">
@@ -2177,7 +2177,7 @@
       <c r="Y10" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="Z10" t="n" s="12">
         <v>483.0</v>
       </c>
       <c r="AA10" t="n">
@@ -3683,10 +3683,10 @@
       <c r="K22" t="n">
         <v>0.0</v>
       </c>
-      <c r="L22" t="n">
+      <c r="L22" t="n" s="12">
         <v>7.2</v>
       </c>
-      <c r="M22" t="n">
+      <c r="M22" t="n" s="12">
         <v>8.9</v>
       </c>
       <c r="N22" t="n">
@@ -4328,7 +4328,7 @@
       <c r="K27" t="n">
         <v>0.0</v>
       </c>
-      <c r="L27" t="n">
+      <c r="L27" t="n" s="12">
         <v>7.8</v>
       </c>
       <c r="M27" t="n">
@@ -4349,7 +4349,7 @@
       <c r="R27" t="n">
         <v>1.0</v>
       </c>
-      <c r="S27" t="n">
+      <c r="S27" t="n" s="12">
         <v>24.0</v>
       </c>
       <c r="T27" t="n">
@@ -5384,7 +5384,7 @@
       <c r="Y35" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z35" t="n">
+      <c r="Z35" t="n" s="12">
         <v>443.0</v>
       </c>
       <c r="AA35" t="n">
@@ -5864,10 +5864,10 @@
       <c r="M39" t="n">
         <v>1.64</v>
       </c>
-      <c r="N39" t="n">
+      <c r="N39" t="n" s="12">
         <v>158.0</v>
       </c>
-      <c r="O39" t="n">
+      <c r="O39" t="n" s="12">
         <v>104.0</v>
       </c>
       <c r="P39" t="n">
@@ -5900,7 +5900,7 @@
       <c r="Y39" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z39" t="n">
+      <c r="Z39" t="n" s="12">
         <v>410.0</v>
       </c>
       <c r="AA39" t="n">
@@ -6124,7 +6124,7 @@
       <c r="O41" t="n">
         <v>38.0</v>
       </c>
-      <c r="P41" t="n">
+      <c r="P41" t="n" s="12">
         <v>1.8</v>
       </c>
       <c r="Q41" t="n">
@@ -6262,7 +6262,7 @@
       <c r="R42" t="n">
         <v>1.0</v>
       </c>
-      <c r="S42" t="n">
+      <c r="S42" t="n" s="12">
         <v>1.0</v>
       </c>
       <c r="T42" t="n">
@@ -6631,7 +6631,7 @@
       <c r="L45" t="n">
         <v>3.64</v>
       </c>
-      <c r="M45" t="n">
+      <c r="M45" t="n" s="12">
         <v>4.59</v>
       </c>
       <c r="N45" t="n">
@@ -6670,7 +6670,7 @@
       <c r="Y45" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z45" t="n">
+      <c r="Z45" t="n" s="12">
         <v>592.0</v>
       </c>
       <c r="AA45" t="n">
@@ -7276,7 +7276,7 @@
       <c r="L50" t="n">
         <v>1.7</v>
       </c>
-      <c r="M50" t="n">
+      <c r="M50" t="n" s="12">
         <v>3.72</v>
       </c>
       <c r="N50" t="n">
@@ -8671,7 +8671,7 @@
       <c r="B61" t="n">
         <v>1.0</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61" t="n" s="12">
         <v>32.0</v>
       </c>
       <c r="D61" t="n">
@@ -8829,10 +8829,10 @@
       <c r="K62" t="n">
         <v>0.0</v>
       </c>
-      <c r="L62" t="n">
+      <c r="L62" t="n" s="12">
         <v>7.4</v>
       </c>
-      <c r="M62" t="n">
+      <c r="M62" t="n" s="12">
         <v>4.7</v>
       </c>
       <c r="N62" t="n">
@@ -9108,7 +9108,7 @@
       <c r="R64" t="n">
         <v>1.0</v>
       </c>
-      <c r="S64" t="n">
+      <c r="S64" t="n" s="12">
         <v>19.0</v>
       </c>
       <c r="T64" t="n">
@@ -9601,10 +9601,10 @@
       <c r="K68" t="n">
         <v>1.0</v>
       </c>
-      <c r="L68" t="n">
+      <c r="L68" t="n" s="12">
         <v>12.0</v>
       </c>
-      <c r="M68" t="n">
+      <c r="M68" t="n" s="12">
         <v>4.2</v>
       </c>
       <c r="N68" t="n">
@@ -9733,7 +9733,7 @@
       <c r="L69" t="n">
         <v>4.1</v>
       </c>
-      <c r="M69" t="n">
+      <c r="M69" t="n" s="12">
         <v>6.4</v>
       </c>
       <c r="N69" t="n">
@@ -9775,10 +9775,10 @@
       <c r="Z69" t="n">
         <v>240.0</v>
       </c>
-      <c r="AA69" t="n">
+      <c r="AA69" t="n" s="12">
         <v>36.0</v>
       </c>
-      <c r="AB69" t="n">
+      <c r="AB69" t="n" s="12">
         <v>21.0</v>
       </c>
       <c r="AC69" s="8"/>
@@ -9901,7 +9901,7 @@
       <c r="Y70" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z70" t="n">
+      <c r="Z70" t="n" s="12">
         <v>480.0</v>
       </c>
       <c r="AA70" t="n">
@@ -10086,7 +10086,7 @@
       <c r="B72" t="n">
         <v>0.0</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72" t="n" s="12">
         <v>37.0</v>
       </c>
       <c r="D72" t="n">
@@ -10287,7 +10287,7 @@
       <c r="Z73" t="n">
         <v>74.0</v>
       </c>
-      <c r="AA73" t="n">
+      <c r="AA73" t="n" s="12">
         <v>23.0</v>
       </c>
       <c r="AB73" t="n">
@@ -10545,7 +10545,7 @@
       <c r="Z75" t="n">
         <v>164.0</v>
       </c>
-      <c r="AA75" t="n">
+      <c r="AA75" t="n" s="12">
         <v>27.0</v>
       </c>
       <c r="AB75" t="n">
@@ -10674,7 +10674,7 @@
       <c r="Z76" t="n">
         <v>147.0</v>
       </c>
-      <c r="AA76" t="n">
+      <c r="AA76" t="n" s="12">
         <v>23.0</v>
       </c>
       <c r="AB76" t="n">
@@ -11017,7 +11017,7 @@
       <c r="L79" t="n">
         <v>4.0</v>
       </c>
-      <c r="M79" t="n">
+      <c r="M79" t="n" s="12">
         <v>4.2</v>
       </c>
       <c r="N79" t="n">
@@ -11317,7 +11317,7 @@
       <c r="Z81" t="n">
         <v>130.0</v>
       </c>
-      <c r="AA81" t="n">
+      <c r="AA81" t="n" s="12">
         <v>49.0</v>
       </c>
       <c r="AB81" t="n">
@@ -11376,7 +11376,7 @@
       <c r="B82" t="n">
         <v>1.0</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82" t="n" s="12">
         <v>38.0</v>
       </c>
       <c r="D82" t="n">
@@ -11448,7 +11448,7 @@
       <c r="Z82" t="n">
         <v>150.0</v>
       </c>
-      <c r="AA82" t="n">
+      <c r="AA82" t="n" s="12">
         <v>26.0</v>
       </c>
       <c r="AB82" t="n">
@@ -11796,7 +11796,7 @@
       <c r="M85" t="n">
         <v>1.0</v>
       </c>
-      <c r="N85" t="n">
+      <c r="N85" t="n" s="12">
         <v>163.0</v>
       </c>
       <c r="O85" t="n">
@@ -12183,10 +12183,10 @@
       <c r="M88" t="n">
         <v>0.9</v>
       </c>
-      <c r="N88" t="n">
+      <c r="N88" t="n" s="12">
         <v>169.0</v>
       </c>
-      <c r="O88" t="n">
+      <c r="O88" t="n" s="12">
         <v>103.0</v>
       </c>
       <c r="P88" t="n">
@@ -12349,10 +12349,10 @@
         <v>1.0</v>
       </c>
       <c r="Z89" s="8"/>
-      <c r="AA89" t="n">
+      <c r="AA89" t="n" s="12">
         <v>34.0</v>
       </c>
-      <c r="AB89" t="n">
+      <c r="AB89" t="n" s="12">
         <v>21.0</v>
       </c>
       <c r="AC89" t="n">
@@ -13123,7 +13123,7 @@
       <c r="Z95" t="n">
         <v>172.0</v>
       </c>
-      <c r="AA95" t="n">
+      <c r="AA95" t="n" s="12">
         <v>29.0</v>
       </c>
       <c r="AB95" t="n">
@@ -13378,7 +13378,7 @@
       <c r="Y97" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z97" t="n">
+      <c r="Z97" t="n" s="12">
         <v>467.0</v>
       </c>
       <c r="AA97" s="8"/>
@@ -13821,7 +13821,7 @@
       <c r="B101" t="n">
         <v>1.0</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101" t="n" s="12">
         <v>38.0</v>
       </c>
       <c r="D101" t="n">
@@ -14107,7 +14107,7 @@
       <c r="L103" t="n">
         <v>4.6</v>
       </c>
-      <c r="M103" t="n">
+      <c r="M103" t="n" s="12">
         <v>4.1</v>
       </c>
       <c r="N103" t="n">
@@ -14149,7 +14149,7 @@
       <c r="Z103" t="n">
         <v>114.0</v>
       </c>
-      <c r="AA103" t="n">
+      <c r="AA103" t="n" s="12">
         <v>27.0</v>
       </c>
       <c r="AB103" t="n">
@@ -14275,7 +14275,7 @@
       <c r="Y104" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z104" t="n">
+      <c r="Z104" t="n" s="12">
         <v>436.0</v>
       </c>
       <c r="AA104" t="n">
@@ -14598,7 +14598,7 @@
       <c r="C107" t="n">
         <v>51.0</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107" t="n" s="12">
         <v>144.0</v>
       </c>
       <c r="E107" t="n">
@@ -14722,7 +14722,7 @@
       <c r="B108" t="n">
         <v>1.0</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108" t="n" s="12">
         <v>32.0</v>
       </c>
       <c r="D108" t="n">
@@ -14851,7 +14851,7 @@
       <c r="B109" t="n">
         <v>1.0</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109" t="n" s="12">
         <v>78.0</v>
       </c>
       <c r="D109" t="n">
@@ -14923,7 +14923,7 @@
       <c r="Z109" t="n">
         <v>133.0</v>
       </c>
-      <c r="AA109" t="n">
+      <c r="AA109" t="n" s="12">
         <v>24.0</v>
       </c>
       <c r="AB109" t="n">
@@ -15007,10 +15007,10 @@
       <c r="K110" t="n">
         <v>0.0</v>
       </c>
-      <c r="L110" t="n">
+      <c r="L110" t="n" s="12">
         <v>6.9</v>
       </c>
-      <c r="M110" t="n">
+      <c r="M110" t="n" s="12">
         <v>3.9</v>
       </c>
       <c r="N110" t="n">
@@ -15052,7 +15052,7 @@
       <c r="Z110" t="n">
         <v>155.0</v>
       </c>
-      <c r="AA110" t="n">
+      <c r="AA110" t="n" s="12">
         <v>27.0</v>
       </c>
       <c r="AB110" t="n">
@@ -15181,7 +15181,7 @@
       <c r="Z111" t="n">
         <v>192.0</v>
       </c>
-      <c r="AA111" t="n">
+      <c r="AA111" t="n" s="12">
         <v>26.0</v>
       </c>
       <c r="AB111" s="8"/>
@@ -15241,7 +15241,7 @@
       <c r="C112" t="n">
         <v>72.0</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112" t="n" s="12">
         <v>126.0</v>
       </c>
       <c r="E112" t="n">
@@ -15369,7 +15369,7 @@
       <c r="B113" t="n">
         <v>1.0</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113" t="n" s="12">
         <v>22.0</v>
       </c>
       <c r="D113" t="n">
@@ -16016,7 +16016,7 @@
       <c r="B118" t="n">
         <v>1.0</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118" t="n" s="12">
         <v>24.0</v>
       </c>
       <c r="D118" t="n">
@@ -16175,7 +16175,7 @@
       <c r="L119" t="n">
         <v>4.1</v>
       </c>
-      <c r="M119" t="n">
+      <c r="M119" t="n" s="12">
         <v>4.3</v>
       </c>
       <c r="N119" t="n">
@@ -16276,7 +16276,7 @@
       <c r="B120" t="n">
         <v>1.0</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120" t="n" s="12">
         <v>25.0</v>
       </c>
       <c r="D120" t="n">
@@ -16840,7 +16840,7 @@
       <c r="R124" t="n">
         <v>1.0</v>
       </c>
-      <c r="S124" t="n">
+      <c r="S124" t="n" s="12">
         <v>24.0</v>
       </c>
       <c r="T124" t="n">
@@ -16951,7 +16951,7 @@
       <c r="L125" t="n">
         <v>2.3</v>
       </c>
-      <c r="M125" t="n">
+      <c r="M125" t="n" s="12">
         <v>3.9</v>
       </c>
       <c r="N125" t="n">
@@ -16990,7 +16990,7 @@
       <c r="Y125" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z125" t="n">
+      <c r="Z125" t="n" s="12">
         <v>526.0</v>
       </c>
       <c r="AA125" t="n">

</xml_diff>

<commit_message>
Symbols with it's colors are added in first row
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="274">
   <si>
     <t>Пациент</t>
   </si>
@@ -828,6 +828,12 @@
   </si>
   <si>
     <t>лет</t>
+  </si>
+  <si>
+    <t>Пропущенные значения</t>
+  </si>
+  <si>
+    <t>Выбросы</t>
   </si>
 </sst>
 </file>
@@ -1014,8 +1020,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="4.43359375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="23.546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.4921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="8.17578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="4.84375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="7.75390625" customWidth="true" bestFit="true"/>
@@ -1059,7 +1065,14 @@
     <col min="43" max="43" width="4.078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="s" s="8">
+        <v>272</v>
+      </c>
+      <c r="B1" t="s" s="12">
+        <v>273</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" t="s" s="4">
         <v>0</v>

</xml_diff>

<commit_message>
method call for class AorticValveStenosis in Main
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -1494,7 +1494,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView workbookViewId="0" tabSelected="true">
+      <pane ySplit="1.0" state="frozen" topLeftCell="A1" activePane="bottomLeft"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
@@ -6614,7 +6617,7 @@
       <c r="O41" t="n">
         <v>38.0</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" t="s" s="68">
         <v>134</v>
       </c>
       <c r="Q41" t="n">
@@ -8291,7 +8294,7 @@
       <c r="O54" t="n">
         <v>54.0</v>
       </c>
-      <c r="P54" t="s">
+      <c r="P54" t="s" s="48">
         <v>140</v>
       </c>
       <c r="Q54" t="n">

</xml_diff>

<commit_message>
new columns was added in Main, Column.R was changed
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -1833,7 +1833,7 @@
       <c r="AN3" t="s">
         <v>37</v>
       </c>
-      <c r="AO3"/>
+      <c r="AO3" s="8"/>
       <c r="AP3" t="s">
         <v>274</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="AN4" t="s">
         <v>37</v>
       </c>
-      <c r="AO4"/>
+      <c r="AO4" s="8"/>
       <c r="AP4" t="s">
         <v>275</v>
       </c>
@@ -2091,7 +2091,7 @@
       <c r="AN5" t="s">
         <v>37</v>
       </c>
-      <c r="AO5"/>
+      <c r="AO5" s="8"/>
       <c r="AP5" t="s">
         <v>276</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="AN6" t="s">
         <v>37</v>
       </c>
-      <c r="AO6"/>
+      <c r="AO6" s="8"/>
       <c r="AP6" t="s">
         <v>277</v>
       </c>
@@ -2349,7 +2349,7 @@
       <c r="AN7" t="s">
         <v>37</v>
       </c>
-      <c r="AO7"/>
+      <c r="AO7" s="8"/>
       <c r="AP7" t="s">
         <v>278</v>
       </c>
@@ -2478,7 +2478,7 @@
       <c r="AN8" t="s">
         <v>37</v>
       </c>
-      <c r="AO8"/>
+      <c r="AO8" s="8"/>
       <c r="AP8" t="s">
         <v>279</v>
       </c>
@@ -2607,7 +2607,7 @@
       <c r="AN9" t="s">
         <v>37</v>
       </c>
-      <c r="AO9"/>
+      <c r="AO9" s="8"/>
       <c r="AP9" t="s">
         <v>280</v>
       </c>
@@ -2734,7 +2734,7 @@
       <c r="AN10" t="s">
         <v>37</v>
       </c>
-      <c r="AO10"/>
+      <c r="AO10" s="8"/>
       <c r="AP10" t="s">
         <v>158</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="AN11" t="s">
         <v>37</v>
       </c>
-      <c r="AO11"/>
+      <c r="AO11" s="8"/>
       <c r="AP11" t="s">
         <v>281</v>
       </c>
@@ -2992,7 +2992,7 @@
       <c r="AN12" t="s">
         <v>37</v>
       </c>
-      <c r="AO12"/>
+      <c r="AO12" s="8"/>
       <c r="AP12" t="s">
         <v>282</v>
       </c>
@@ -3121,7 +3121,7 @@
       <c r="AN13" t="s">
         <v>37</v>
       </c>
-      <c r="AO13"/>
+      <c r="AO13" s="8"/>
       <c r="AP13" t="s">
         <v>283</v>
       </c>
@@ -3250,7 +3250,7 @@
       <c r="AN14" t="s">
         <v>37</v>
       </c>
-      <c r="AO14"/>
+      <c r="AO14" s="8"/>
       <c r="AP14" t="s">
         <v>284</v>
       </c>
@@ -3379,7 +3379,7 @@
       <c r="AN15" t="s">
         <v>37</v>
       </c>
-      <c r="AO15"/>
+      <c r="AO15" s="8"/>
       <c r="AP15" t="s">
         <v>285</v>
       </c>
@@ -3508,7 +3508,7 @@
       <c r="AN16" t="s">
         <v>37</v>
       </c>
-      <c r="AO16"/>
+      <c r="AO16" s="8"/>
       <c r="AP16" t="s">
         <v>286</v>
       </c>
@@ -3637,7 +3637,7 @@
       <c r="AN17" t="s">
         <v>37</v>
       </c>
-      <c r="AO17"/>
+      <c r="AO17" s="8"/>
       <c r="AP17" t="s">
         <v>287</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="AN18" t="s">
         <v>37</v>
       </c>
-      <c r="AO18"/>
+      <c r="AO18" s="8"/>
       <c r="AP18" t="s">
         <v>288</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="AN19" t="s">
         <v>37</v>
       </c>
-      <c r="AO19"/>
+      <c r="AO19" s="8"/>
       <c r="AP19" t="s">
         <v>289</v>
       </c>
@@ -4024,7 +4024,7 @@
       <c r="AN20" t="s">
         <v>37</v>
       </c>
-      <c r="AO20"/>
+      <c r="AO20" s="8"/>
       <c r="AP20" t="s">
         <v>290</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="AN21" t="s">
         <v>37</v>
       </c>
-      <c r="AO21"/>
+      <c r="AO21" s="8"/>
       <c r="AP21" t="s">
         <v>291</v>
       </c>
@@ -4282,7 +4282,7 @@
       <c r="AN22" t="s">
         <v>37</v>
       </c>
-      <c r="AO22"/>
+      <c r="AO22" s="8"/>
       <c r="AP22" t="s">
         <v>240</v>
       </c>
@@ -4411,7 +4411,7 @@
       <c r="AN23" t="s">
         <v>37</v>
       </c>
-      <c r="AO23"/>
+      <c r="AO23" s="8"/>
       <c r="AP23" t="s">
         <v>292</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="AN24" t="s">
         <v>37</v>
       </c>
-      <c r="AO24"/>
+      <c r="AO24" s="8"/>
       <c r="AP24" t="s">
         <v>293</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="AN25" t="s">
         <v>37</v>
       </c>
-      <c r="AO25"/>
+      <c r="AO25" s="8"/>
       <c r="AP25" t="s">
         <v>294</v>
       </c>
@@ -4798,7 +4798,7 @@
       <c r="AN26" t="s">
         <v>37</v>
       </c>
-      <c r="AO26"/>
+      <c r="AO26" s="8"/>
       <c r="AP26" t="s">
         <v>295</v>
       </c>
@@ -4923,7 +4923,7 @@
       <c r="AN27" t="s">
         <v>37</v>
       </c>
-      <c r="AO27"/>
+      <c r="AO27" s="8"/>
       <c r="AP27" t="s">
         <v>296</v>
       </c>
@@ -5052,7 +5052,7 @@
       <c r="AN28" t="s">
         <v>37</v>
       </c>
-      <c r="AO28"/>
+      <c r="AO28" s="8"/>
       <c r="AP28" t="s">
         <v>297</v>
       </c>
@@ -5179,7 +5179,7 @@
       <c r="AN29" t="s">
         <v>37</v>
       </c>
-      <c r="AO29"/>
+      <c r="AO29" s="8"/>
       <c r="AP29" t="s">
         <v>298</v>
       </c>
@@ -5306,7 +5306,7 @@
       <c r="AN30" t="s">
         <v>37</v>
       </c>
-      <c r="AO30"/>
+      <c r="AO30" s="8"/>
       <c r="AP30" t="s">
         <v>299</v>
       </c>
@@ -5435,7 +5435,7 @@
       <c r="AN31" t="s">
         <v>37</v>
       </c>
-      <c r="AO31"/>
+      <c r="AO31" s="8"/>
       <c r="AP31" t="s">
         <v>300</v>
       </c>
@@ -5564,7 +5564,7 @@
       <c r="AN32" t="s">
         <v>37</v>
       </c>
-      <c r="AO32"/>
+      <c r="AO32" s="8"/>
       <c r="AP32" t="s">
         <v>301</v>
       </c>
@@ -5693,7 +5693,7 @@
       <c r="AN33" t="s">
         <v>37</v>
       </c>
-      <c r="AO33"/>
+      <c r="AO33" s="8"/>
       <c r="AP33" t="s">
         <v>302</v>
       </c>
@@ -5784,7 +5784,7 @@
       <c r="AB34" s="8"/>
       <c r="AC34"/>
       <c r="AD34"/>
-      <c r="AE34"/>
+      <c r="AE34" s="8"/>
       <c r="AF34" t="n">
         <v>1.0</v>
       </c>
@@ -5812,7 +5812,7 @@
       <c r="AN34" t="s">
         <v>37</v>
       </c>
-      <c r="AO34"/>
+      <c r="AO34" s="8"/>
       <c r="AP34" t="s">
         <v>303</v>
       </c>
@@ -5941,7 +5941,7 @@
       <c r="AN35" t="s">
         <v>37</v>
       </c>
-      <c r="AO35"/>
+      <c r="AO35" s="8"/>
       <c r="AP35" t="s">
         <v>304</v>
       </c>
@@ -6070,7 +6070,7 @@
       <c r="AN36" t="s">
         <v>37</v>
       </c>
-      <c r="AO36"/>
+      <c r="AO36" s="8"/>
       <c r="AP36" t="s">
         <v>215</v>
       </c>
@@ -6199,7 +6199,7 @@
       <c r="AN37" t="s">
         <v>37</v>
       </c>
-      <c r="AO37"/>
+      <c r="AO37" s="8"/>
       <c r="AP37" t="s">
         <v>305</v>
       </c>
@@ -6328,7 +6328,7 @@
       <c r="AN38" t="s">
         <v>37</v>
       </c>
-      <c r="AO38"/>
+      <c r="AO38" s="8"/>
       <c r="AP38" t="s">
         <v>306</v>
       </c>
@@ -6453,7 +6453,7 @@
       <c r="AN39" t="s">
         <v>37</v>
       </c>
-      <c r="AO39"/>
+      <c r="AO39" s="8"/>
       <c r="AP39" t="s">
         <v>307</v>
       </c>
@@ -6582,7 +6582,7 @@
       <c r="AN40" t="s">
         <v>37</v>
       </c>
-      <c r="AO40"/>
+      <c r="AO40" s="8"/>
       <c r="AP40" t="s">
         <v>308</v>
       </c>
@@ -6711,7 +6711,7 @@
       <c r="AN41" t="s">
         <v>37</v>
       </c>
-      <c r="AO41"/>
+      <c r="AO41" s="8"/>
       <c r="AP41" t="s">
         <v>309</v>
       </c>
@@ -6840,7 +6840,7 @@
       <c r="AN42" t="s">
         <v>37</v>
       </c>
-      <c r="AO42"/>
+      <c r="AO42" s="8"/>
       <c r="AP42" t="s">
         <v>310</v>
       </c>
@@ -6969,7 +6969,7 @@
       <c r="AN43" t="s">
         <v>37</v>
       </c>
-      <c r="AO43"/>
+      <c r="AO43" s="8"/>
       <c r="AP43" t="s">
         <v>311</v>
       </c>
@@ -7098,7 +7098,7 @@
       <c r="AN44" t="s">
         <v>37</v>
       </c>
-      <c r="AO44"/>
+      <c r="AO44" s="8"/>
       <c r="AP44" t="s">
         <v>312</v>
       </c>
@@ -7227,7 +7227,7 @@
       <c r="AN45" t="s">
         <v>37</v>
       </c>
-      <c r="AO45"/>
+      <c r="AO45" s="8"/>
       <c r="AP45" t="s">
         <v>313</v>
       </c>
@@ -7356,7 +7356,7 @@
       <c r="AN46" t="s">
         <v>37</v>
       </c>
-      <c r="AO46"/>
+      <c r="AO46" s="8"/>
       <c r="AP46" t="s">
         <v>314</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="AN47" t="s">
         <v>37</v>
       </c>
-      <c r="AO47"/>
+      <c r="AO47" s="8"/>
       <c r="AP47" t="s">
         <v>315</v>
       </c>
@@ -7614,7 +7614,7 @@
       <c r="AN48" t="s">
         <v>37</v>
       </c>
-      <c r="AO48"/>
+      <c r="AO48" s="8"/>
       <c r="AP48" t="s">
         <v>195</v>
       </c>
@@ -7743,7 +7743,7 @@
       <c r="AN49" t="s">
         <v>37</v>
       </c>
-      <c r="AO49"/>
+      <c r="AO49" s="8"/>
       <c r="AP49" t="s">
         <v>196</v>
       </c>
@@ -7872,7 +7872,7 @@
       <c r="AN50" t="s">
         <v>37</v>
       </c>
-      <c r="AO50"/>
+      <c r="AO50" s="8"/>
       <c r="AP50" t="s">
         <v>316</v>
       </c>
@@ -8001,7 +8001,7 @@
       <c r="AN51" t="s">
         <v>37</v>
       </c>
-      <c r="AO51"/>
+      <c r="AO51" s="8"/>
       <c r="AP51" t="s">
         <v>317</v>
       </c>
@@ -8130,7 +8130,7 @@
       <c r="AN52" t="s">
         <v>37</v>
       </c>
-      <c r="AO52"/>
+      <c r="AO52" s="8"/>
       <c r="AP52" t="s">
         <v>318</v>
       </c>
@@ -8259,7 +8259,7 @@
       <c r="AN53" t="s">
         <v>37</v>
       </c>
-      <c r="AO53"/>
+      <c r="AO53" s="8"/>
       <c r="AP53" t="s">
         <v>319</v>
       </c>
@@ -9019,7 +9019,7 @@
       <c r="AH59" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI59" t="n">
+      <c r="AI59" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ59" t="n">
@@ -10309,7 +10309,7 @@
       <c r="AH69" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI69" t="n">
+      <c r="AI69" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ69" t="n">
@@ -11722,7 +11722,7 @@
       <c r="AH80" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI80" t="n">
+      <c r="AI80" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ80" t="n">
@@ -12498,7 +12498,7 @@
       <c r="AH86" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI86" t="n">
+      <c r="AI86" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ86" t="n">
@@ -13907,7 +13907,7 @@
       <c r="AH97" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI97" t="n">
+      <c r="AI97" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ97" t="n">
@@ -15709,7 +15709,7 @@
       <c r="AH111" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI111" t="n">
+      <c r="AI111" t="n" s="48">
         <v>2.0</v>
       </c>
       <c r="AJ111" t="n">

</xml_diff>

<commit_message>
method for checking consecutive dates was created and now good works
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="302">
   <si>
     <t>Пациент</t>
   </si>
@@ -578,7 +578,7 @@
     <t>des_bms</t>
   </si>
   <si>
-    <t>20.02.2010</t>
+    <t>20.02.2008</t>
   </si>
   <si>
     <t>09.05.2009</t>
@@ -915,6 +915,9 @@
   </si>
   <si>
     <t>Выбросы</t>
+  </si>
+  <si>
+    <t>Непоследовательные даты</t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="18">
+  <fonts count="27">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -1015,8 +1018,53 @@
       <sz val="11.0"/>
       <i val="true"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <i val="true"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1088,6 +1136,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF3030"/>
+        <bgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="CDBE70"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor rgb="CDBE70"/>
+        <bgColor rgb="ADD8E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="CDBE70"/>
         <bgColor rgb="ADD8E6"/>
       </patternFill>
     </fill>
@@ -1172,7 +1237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -1200,52 +1265,88 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1265,7 +1366,7 @@
     <col min="2" max="2" width="13.3125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.67578125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.4921875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="7.75390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="27.87890625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="14.89453125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="11.87890625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="5.58984375" customWidth="true" bestFit="true"/>
@@ -1302,7 +1403,7 @@
     <col min="39" max="39" width="14.83984375" customWidth="true" bestFit="true"/>
     <col min="40" max="40" width="11.05859375" customWidth="true" bestFit="true"/>
     <col min="41" max="41" width="23.390625" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="10.98828125" customWidth="true" bestFit="true"/>
+    <col min="42" max="42" width="11.10546875" customWidth="true" bestFit="true"/>
     <col min="43" max="43" width="4.078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -1310,14 +1411,17 @@
       <c r="A1" t="s" s="8">
         <v>297</v>
       </c>
-      <c r="B1" t="s" s="28">
+      <c r="B1" t="s" s="32">
         <v>298</v>
       </c>
-      <c r="C1" t="s" s="48">
+      <c r="C1" t="s" s="56">
         <v>299</v>
       </c>
-      <c r="D1" t="s" s="68">
+      <c r="D1" t="s" s="80">
         <v>300</v>
+      </c>
+      <c r="E1" t="s" s="104">
+        <v>301</v>
       </c>
     </row>
     <row r="2">
@@ -1455,7 +1559,7 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" t="s" s="28">
+      <c r="B3" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C3" t="n">
@@ -1521,7 +1625,7 @@
       <c r="W3" t="n">
         <v>0.0</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" t="s" s="104">
         <v>65</v>
       </c>
       <c r="Y3" t="n">
@@ -1573,7 +1677,7 @@
         <v>37</v>
       </c>
       <c r="AO3" s="8"/>
-      <c r="AP3" t="s">
+      <c r="AP3" t="s" s="104">
         <v>188</v>
       </c>
       <c r="AQ3" t="s">
@@ -1584,7 +1688,7 @@
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" t="s" s="28">
+      <c r="B4" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C4" t="n">
@@ -1656,7 +1760,7 @@
       <c r="Y4" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z4" t="n" s="68">
+      <c r="Z4" t="n" s="80">
         <v>434.0</v>
       </c>
       <c r="AA4" t="n">
@@ -1713,7 +1817,7 @@
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" t="s" s="28">
+      <c r="B5" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C5" t="n">
@@ -1779,7 +1883,7 @@
       <c r="W5" t="n">
         <v>0.0</v>
       </c>
-      <c r="X5" t="s" s="28">
+      <c r="X5" t="s" s="32">
         <v>67</v>
       </c>
       <c r="Y5" t="n">
@@ -1842,10 +1946,10 @@
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" t="s" s="28">
+      <c r="B6" t="s" s="32">
         <v>40</v>
       </c>
-      <c r="C6" t="n" s="68">
+      <c r="C6" t="n" s="80">
         <v>37.0</v>
       </c>
       <c r="D6" t="n">
@@ -1914,7 +2018,7 @@
       <c r="Y6" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z6" t="n" s="68">
+      <c r="Z6" t="n" s="80">
         <v>410.0</v>
       </c>
       <c r="AA6" t="n">
@@ -1971,7 +2075,7 @@
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s" s="28">
+      <c r="B7" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C7" t="n">
@@ -2100,7 +2204,7 @@
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s" s="28">
+      <c r="B8" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C8" t="n">
@@ -2229,7 +2333,7 @@
       <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s" s="28">
+      <c r="B9" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C9" t="n">
@@ -2358,7 +2462,7 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s" s="28">
+      <c r="B10" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C10" t="n">
@@ -2430,7 +2534,7 @@
       <c r="Y10" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z10" t="n" s="68">
+      <c r="Z10" t="n" s="80">
         <v>483.0</v>
       </c>
       <c r="AA10" t="n">
@@ -2487,7 +2591,7 @@
       <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s" s="28">
+      <c r="B11" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C11" t="n">
@@ -2616,7 +2720,7 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="s" s="28">
+      <c r="B12" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C12" t="n">
@@ -2745,7 +2849,7 @@
       <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s" s="28">
+      <c r="B13" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C13" t="n">
@@ -2874,7 +2978,7 @@
       <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s" s="28">
+      <c r="B14" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C14" t="n">
@@ -3003,7 +3107,7 @@
       <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s" s="28">
+      <c r="B15" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C15" t="n">
@@ -3132,7 +3236,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s" s="28">
+      <c r="B16" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C16" t="n">
@@ -3261,7 +3365,7 @@
       <c r="A17" t="s">
         <v>38</v>
       </c>
-      <c r="B17" t="s" s="28">
+      <c r="B17" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C17" t="n">
@@ -3390,7 +3494,7 @@
       <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s" s="28">
+      <c r="B18" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C18" t="n">
@@ -3519,7 +3623,7 @@
       <c r="A19" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s" s="28">
+      <c r="B19" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C19" t="n">
@@ -3648,7 +3752,7 @@
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s" s="28">
+      <c r="B20" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C20" t="n">
@@ -3777,7 +3881,7 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" t="s" s="28">
+      <c r="B21" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C21" t="n">
@@ -3906,7 +4010,7 @@
       <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B22" t="s" s="28">
+      <c r="B22" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C22" t="n">
@@ -3936,10 +4040,10 @@
       <c r="K22" t="n">
         <v>0.0</v>
       </c>
-      <c r="L22" t="n" s="68">
+      <c r="L22" t="n" s="80">
         <v>7.2</v>
       </c>
-      <c r="M22" t="n" s="68">
+      <c r="M22" t="n" s="80">
         <v>8.9</v>
       </c>
       <c r="N22" t="n">
@@ -4035,7 +4139,7 @@
       <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B23" t="s" s="28">
+      <c r="B23" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C23" t="n">
@@ -4164,7 +4268,7 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s" s="28">
+      <c r="B24" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C24" t="n">
@@ -4293,7 +4397,7 @@
       <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s" s="28">
+      <c r="B25" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C25" t="n">
@@ -4422,7 +4526,7 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" t="s" s="28">
+      <c r="B26" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C26" t="n">
@@ -4551,7 +4655,7 @@
       <c r="A27" t="s">
         <v>38</v>
       </c>
-      <c r="B27" t="s" s="28">
+      <c r="B27" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C27" t="n">
@@ -4581,7 +4685,7 @@
       <c r="K27" t="n">
         <v>0.0</v>
       </c>
-      <c r="L27" t="n" s="68">
+      <c r="L27" t="n" s="80">
         <v>7.8</v>
       </c>
       <c r="M27" t="n">
@@ -4602,7 +4706,7 @@
       <c r="R27" t="n">
         <v>1.0</v>
       </c>
-      <c r="S27" t="n" s="68">
+      <c r="S27" t="n" s="80">
         <v>24.0</v>
       </c>
       <c r="T27" t="n">
@@ -4617,7 +4721,7 @@
       <c r="W27" t="n">
         <v>2.0</v>
       </c>
-      <c r="X27" t="s">
+      <c r="X27" t="s" s="104">
         <v>89</v>
       </c>
       <c r="Y27" t="n">
@@ -4665,7 +4769,7 @@
         <v>37</v>
       </c>
       <c r="AO27" s="8"/>
-      <c r="AP27" t="s">
+      <c r="AP27" t="s" s="104">
         <v>209</v>
       </c>
       <c r="AQ27" t="s">
@@ -4676,7 +4780,7 @@
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s" s="28">
+      <c r="B28" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C28" t="n">
@@ -4805,7 +4909,7 @@
       <c r="A29" t="s">
         <v>38</v>
       </c>
-      <c r="B29" t="s" s="28">
+      <c r="B29" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C29" t="n">
@@ -4932,7 +5036,7 @@
       <c r="A30" t="s">
         <v>38</v>
       </c>
-      <c r="B30" t="s" s="28">
+      <c r="B30" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C30" t="n">
@@ -5059,7 +5163,7 @@
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s" s="28">
+      <c r="B31" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C31" t="n">
@@ -5188,7 +5292,7 @@
       <c r="A32" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="s" s="28">
+      <c r="B32" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C32" t="n">
@@ -5317,7 +5421,7 @@
       <c r="A33" t="s">
         <v>38</v>
       </c>
-      <c r="B33" t="s" s="28">
+      <c r="B33" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C33" t="n">
@@ -5446,7 +5550,7 @@
       <c r="A34" t="s">
         <v>38</v>
       </c>
-      <c r="B34" t="s" s="28">
+      <c r="B34" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C34" t="n">
@@ -5565,7 +5669,7 @@
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35" t="s" s="28">
+      <c r="B35" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C35" t="n">
@@ -5637,7 +5741,7 @@
       <c r="Y35" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z35" t="n" s="68">
+      <c r="Z35" t="n" s="80">
         <v>443.0</v>
       </c>
       <c r="AA35" t="n">
@@ -5694,7 +5798,7 @@
       <c r="A36" t="s">
         <v>38</v>
       </c>
-      <c r="B36" t="s" s="28">
+      <c r="B36" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C36" t="n">
@@ -5823,7 +5927,7 @@
       <c r="A37" t="s">
         <v>38</v>
       </c>
-      <c r="B37" t="s" s="28">
+      <c r="B37" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C37" t="n">
@@ -5952,7 +6056,7 @@
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s" s="28">
+      <c r="B38" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C38" t="n">
@@ -5961,7 +6065,7 @@
       <c r="D38" t="n">
         <v>57.0</v>
       </c>
-      <c r="E38" t="s" s="28">
+      <c r="E38" t="s" s="32">
         <v>40</v>
       </c>
       <c r="F38" t="n">
@@ -6081,7 +6185,7 @@
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" t="s" s="28">
+      <c r="B39" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C39" t="n">
@@ -6117,10 +6221,10 @@
       <c r="M39" t="n">
         <v>1.64</v>
       </c>
-      <c r="N39" t="n" s="68">
+      <c r="N39" t="n" s="80">
         <v>158.0</v>
       </c>
-      <c r="O39" t="n" s="68">
+      <c r="O39" t="n" s="80">
         <v>104.0</v>
       </c>
       <c r="P39" t="s">
@@ -6153,7 +6257,7 @@
       <c r="Y39" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z39" t="n" s="68">
+      <c r="Z39" t="n" s="80">
         <v>410.0</v>
       </c>
       <c r="AA39" t="n">
@@ -6206,7 +6310,7 @@
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s" s="28">
+      <c r="B40" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C40" t="n">
@@ -6335,7 +6439,7 @@
       <c r="A41" t="s">
         <v>38</v>
       </c>
-      <c r="B41" t="s" s="28">
+      <c r="B41" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C41" t="n">
@@ -6377,7 +6481,7 @@
       <c r="O41" t="n">
         <v>38.0</v>
       </c>
-      <c r="P41" t="s" s="68">
+      <c r="P41" t="s" s="80">
         <v>57</v>
       </c>
       <c r="Q41" t="n">
@@ -6464,7 +6568,7 @@
       <c r="A42" t="s">
         <v>38</v>
       </c>
-      <c r="B42" t="s" s="28">
+      <c r="B42" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C42" t="n">
@@ -6515,7 +6619,7 @@
       <c r="R42" t="n">
         <v>1.0</v>
       </c>
-      <c r="S42" t="n" s="68">
+      <c r="S42" t="n" s="80">
         <v>1.0</v>
       </c>
       <c r="T42" t="n">
@@ -6593,7 +6697,7 @@
       <c r="A43" t="s">
         <v>38</v>
       </c>
-      <c r="B43" t="s" s="28">
+      <c r="B43" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C43" t="n">
@@ -6722,7 +6826,7 @@
       <c r="A44" t="s">
         <v>38</v>
       </c>
-      <c r="B44" t="s" s="28">
+      <c r="B44" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C44" t="n">
@@ -6851,7 +6955,7 @@
       <c r="A45" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s" s="28">
+      <c r="B45" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C45" t="n">
@@ -6860,7 +6964,7 @@
       <c r="D45" t="n">
         <v>73.0</v>
       </c>
-      <c r="E45" t="s" s="28">
+      <c r="E45" t="s" s="32">
         <v>40</v>
       </c>
       <c r="F45" t="n">
@@ -6884,7 +6988,7 @@
       <c r="L45" t="n">
         <v>3.64</v>
       </c>
-      <c r="M45" t="n" s="68">
+      <c r="M45" t="n" s="80">
         <v>4.59</v>
       </c>
       <c r="N45" t="n">
@@ -6923,7 +7027,7 @@
       <c r="Y45" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z45" t="n" s="68">
+      <c r="Z45" t="n" s="80">
         <v>592.0</v>
       </c>
       <c r="AA45" t="n">
@@ -6980,7 +7084,7 @@
       <c r="A46" t="s">
         <v>38</v>
       </c>
-      <c r="B46" t="s" s="28">
+      <c r="B46" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C46" t="n">
@@ -7109,7 +7213,7 @@
       <c r="A47" t="s">
         <v>38</v>
       </c>
-      <c r="B47" t="s" s="28">
+      <c r="B47" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C47" t="n">
@@ -7238,7 +7342,7 @@
       <c r="A48" t="s">
         <v>38</v>
       </c>
-      <c r="B48" t="s" s="28">
+      <c r="B48" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C48" t="n">
@@ -7367,7 +7471,7 @@
       <c r="A49" t="s">
         <v>38</v>
       </c>
-      <c r="B49" t="s" s="28">
+      <c r="B49" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C49" t="n">
@@ -7496,7 +7600,7 @@
       <c r="A50" t="s">
         <v>38</v>
       </c>
-      <c r="B50" t="s" s="28">
+      <c r="B50" t="s" s="32">
         <v>41</v>
       </c>
       <c r="C50" t="n">
@@ -7529,7 +7633,7 @@
       <c r="L50" t="n">
         <v>1.7</v>
       </c>
-      <c r="M50" t="n" s="68">
+      <c r="M50" t="n" s="80">
         <v>3.72</v>
       </c>
       <c r="N50" t="n">
@@ -7625,7 +7729,7 @@
       <c r="A51" t="s">
         <v>38</v>
       </c>
-      <c r="B51" t="s" s="28">
+      <c r="B51" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C51" t="n">
@@ -7754,7 +7858,7 @@
       <c r="A52" t="s">
         <v>38</v>
       </c>
-      <c r="B52" t="s" s="28">
+      <c r="B52" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C52" t="n">
@@ -7883,7 +7987,7 @@
       <c r="A53" t="s">
         <v>38</v>
       </c>
-      <c r="B53" t="s" s="28">
+      <c r="B53" t="s" s="32">
         <v>40</v>
       </c>
       <c r="C53" t="n">
@@ -8054,7 +8158,7 @@
       <c r="O54" t="n">
         <v>54.0</v>
       </c>
-      <c r="P54" t="s" s="28">
+      <c r="P54" t="s" s="32">
         <v>63</v>
       </c>
       <c r="Q54" t="n">
@@ -8576,7 +8680,7 @@
       <c r="O58" t="n">
         <v>76.0</v>
       </c>
-      <c r="P58" t="s" s="28">
+      <c r="P58" t="s" s="32">
         <v>47</v>
       </c>
       <c r="Q58" t="n">
@@ -8708,7 +8812,7 @@
       <c r="P59" t="s">
         <v>49</v>
       </c>
-      <c r="Q59" t="n" s="48">
+      <c r="Q59" t="n" s="56">
         <v>3.0</v>
       </c>
       <c r="R59" t="n">
@@ -8760,7 +8864,7 @@
       <c r="AH59" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI59" t="n" s="28">
+      <c r="AI59" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ59" t="n">
@@ -8924,7 +9028,7 @@
       <c r="B61" t="s">
         <v>40</v>
       </c>
-      <c r="C61" t="n" s="68">
+      <c r="C61" t="n" s="80">
         <v>32.0</v>
       </c>
       <c r="D61" t="n">
@@ -9082,10 +9186,10 @@
       <c r="K62" t="n">
         <v>0.0</v>
       </c>
-      <c r="L62" t="n" s="68">
+      <c r="L62" t="n" s="80">
         <v>7.4</v>
       </c>
-      <c r="M62" t="n" s="68">
+      <c r="M62" t="n" s="80">
         <v>4.7</v>
       </c>
       <c r="N62" t="n">
@@ -9340,7 +9444,7 @@
       <c r="K64" t="n">
         <v>0.0</v>
       </c>
-      <c r="L64" t="n" s="68">
+      <c r="L64" t="n" s="80">
         <v>6.2</v>
       </c>
       <c r="M64" t="n">
@@ -9361,7 +9465,7 @@
       <c r="R64" t="n">
         <v>1.0</v>
       </c>
-      <c r="S64" t="n" s="68">
+      <c r="S64" t="n" s="80">
         <v>19.0</v>
       </c>
       <c r="T64" t="n">
@@ -9854,10 +9958,10 @@
       <c r="K68" t="n">
         <v>1.0</v>
       </c>
-      <c r="L68" t="n" s="68">
+      <c r="L68" t="n" s="80">
         <v>12.0</v>
       </c>
-      <c r="M68" t="n" s="68">
+      <c r="M68" t="n" s="80">
         <v>4.2</v>
       </c>
       <c r="N68" t="n">
@@ -9986,7 +10090,7 @@
       <c r="L69" t="n">
         <v>4.1</v>
       </c>
-      <c r="M69" t="n" s="68">
+      <c r="M69" t="n" s="80">
         <v>6.4</v>
       </c>
       <c r="N69" t="n">
@@ -10028,10 +10132,10 @@
       <c r="Z69" t="n">
         <v>240.0</v>
       </c>
-      <c r="AA69" t="n" s="68">
+      <c r="AA69" t="n" s="80">
         <v>36.0</v>
       </c>
-      <c r="AB69" t="n" s="68">
+      <c r="AB69" t="n" s="80">
         <v>21.0</v>
       </c>
       <c r="AC69" s="8"/>
@@ -10050,7 +10154,7 @@
       <c r="AH69" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI69" t="n" s="28">
+      <c r="AI69" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ69" t="n">
@@ -10154,7 +10258,7 @@
       <c r="Y70" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z70" t="n" s="68">
+      <c r="Z70" t="n" s="80">
         <v>480.0</v>
       </c>
       <c r="AA70" t="n">
@@ -10339,7 +10443,7 @@
       <c r="B72" t="s">
         <v>41</v>
       </c>
-      <c r="C72" t="n" s="68">
+      <c r="C72" t="n" s="80">
         <v>37.0</v>
       </c>
       <c r="D72" t="n">
@@ -10540,7 +10644,7 @@
       <c r="Z73" t="n">
         <v>74.0</v>
       </c>
-      <c r="AA73" t="n" s="68">
+      <c r="AA73" t="n" s="80">
         <v>23.0</v>
       </c>
       <c r="AB73" t="n">
@@ -10798,7 +10902,7 @@
       <c r="Z75" t="n">
         <v>164.0</v>
       </c>
-      <c r="AA75" t="n" s="68">
+      <c r="AA75" t="n" s="80">
         <v>27.0</v>
       </c>
       <c r="AB75" t="n">
@@ -10927,7 +11031,7 @@
       <c r="Z76" t="n">
         <v>147.0</v>
       </c>
-      <c r="AA76" t="n" s="68">
+      <c r="AA76" t="n" s="80">
         <v>23.0</v>
       </c>
       <c r="AB76" t="n">
@@ -11270,7 +11374,7 @@
       <c r="L79" t="n">
         <v>4.0</v>
       </c>
-      <c r="M79" t="n" s="68">
+      <c r="M79" t="n" s="80">
         <v>4.2</v>
       </c>
       <c r="N79" t="n">
@@ -11349,7 +11453,7 @@
       <c r="AM79" t="n">
         <v>2.0</v>
       </c>
-      <c r="AN79" t="s" s="48">
+      <c r="AN79" t="s" s="56">
         <v>186</v>
       </c>
       <c r="AO79" t="n">
@@ -11408,7 +11512,7 @@
       <c r="O80" t="n">
         <v>85.0</v>
       </c>
-      <c r="P80" t="s" s="28">
+      <c r="P80" t="s" s="32">
         <v>61</v>
       </c>
       <c r="Q80" t="n">
@@ -11463,7 +11567,7 @@
       <c r="AH80" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI80" t="n" s="28">
+      <c r="AI80" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ80" t="n">
@@ -11570,7 +11674,7 @@
       <c r="Z81" t="n">
         <v>130.0</v>
       </c>
-      <c r="AA81" t="n" s="68">
+      <c r="AA81" t="n" s="80">
         <v>49.0</v>
       </c>
       <c r="AB81" t="n">
@@ -11629,7 +11733,7 @@
       <c r="B82" t="s">
         <v>40</v>
       </c>
-      <c r="C82" t="n" s="68">
+      <c r="C82" t="n" s="80">
         <v>38.0</v>
       </c>
       <c r="D82" t="n">
@@ -11701,7 +11805,7 @@
       <c r="Z82" t="n">
         <v>150.0</v>
       </c>
-      <c r="AA82" t="n" s="68">
+      <c r="AA82" t="n" s="80">
         <v>26.0</v>
       </c>
       <c r="AB82" t="n">
@@ -12049,7 +12153,7 @@
       <c r="M85" t="n">
         <v>1.0</v>
       </c>
-      <c r="N85" t="n" s="68">
+      <c r="N85" t="n" s="80">
         <v>163.0</v>
       </c>
       <c r="O85" t="n">
@@ -12239,7 +12343,7 @@
       <c r="AH86" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI86" t="n" s="28">
+      <c r="AI86" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ86" t="n">
@@ -12436,10 +12540,10 @@
       <c r="M88" t="n">
         <v>0.9</v>
       </c>
-      <c r="N88" t="n" s="68">
+      <c r="N88" t="n" s="80">
         <v>169.0</v>
       </c>
-      <c r="O88" t="n" s="68">
+      <c r="O88" t="n" s="80">
         <v>103.0</v>
       </c>
       <c r="P88" t="s">
@@ -12602,10 +12706,10 @@
         <v>1.0</v>
       </c>
       <c r="Z89" s="8"/>
-      <c r="AA89" t="n" s="68">
+      <c r="AA89" t="n" s="80">
         <v>34.0</v>
       </c>
-      <c r="AB89" t="n" s="68">
+      <c r="AB89" t="n" s="80">
         <v>21.0</v>
       </c>
       <c r="AC89" t="n">
@@ -13376,7 +13480,7 @@
       <c r="Z95" t="n">
         <v>172.0</v>
       </c>
-      <c r="AA95" t="n" s="68">
+      <c r="AA95" t="n" s="80">
         <v>29.0</v>
       </c>
       <c r="AB95" t="n">
@@ -13625,7 +13729,7 @@
       <c r="Y97" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z97" t="n" s="68">
+      <c r="Z97" t="n" s="80">
         <v>467.0</v>
       </c>
       <c r="AA97" s="8"/>
@@ -13648,7 +13752,7 @@
       <c r="AH97" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI97" t="n" s="28">
+      <c r="AI97" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ97" t="n">
@@ -13663,7 +13767,7 @@
       <c r="AM97" t="n">
         <v>0.0</v>
       </c>
-      <c r="AN97" t="s" s="48">
+      <c r="AN97" t="s" s="56">
         <v>187</v>
       </c>
       <c r="AO97" t="n">
@@ -13719,7 +13823,7 @@
       <c r="N98" t="n">
         <v>138.0</v>
       </c>
-      <c r="O98" t="n" s="68">
+      <c r="O98" t="n" s="80">
         <v>90.0</v>
       </c>
       <c r="P98" t="s">
@@ -14068,7 +14172,7 @@
       <c r="B101" t="s">
         <v>40</v>
       </c>
-      <c r="C101" t="n" s="68">
+      <c r="C101" t="n" s="80">
         <v>38.0</v>
       </c>
       <c r="D101" t="n">
@@ -14354,7 +14458,7 @@
       <c r="L103" t="n">
         <v>4.6</v>
       </c>
-      <c r="M103" t="n" s="68">
+      <c r="M103" t="n" s="80">
         <v>4.1</v>
       </c>
       <c r="N103" t="n">
@@ -14396,7 +14500,7 @@
       <c r="Z103" t="n">
         <v>114.0</v>
       </c>
-      <c r="AA103" t="n" s="68">
+      <c r="AA103" t="n" s="80">
         <v>27.0</v>
       </c>
       <c r="AB103" t="n">
@@ -14522,7 +14626,7 @@
       <c r="Y104" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z104" t="n" s="68">
+      <c r="Z104" t="n" s="80">
         <v>436.0</v>
       </c>
       <c r="AA104" t="n">
@@ -14845,7 +14949,7 @@
       <c r="C107" t="n">
         <v>51.0</v>
       </c>
-      <c r="D107" t="n" s="68">
+      <c r="D107" t="n" s="80">
         <v>144.0</v>
       </c>
       <c r="E107" t="s">
@@ -14969,7 +15073,7 @@
       <c r="B108" t="s">
         <v>40</v>
       </c>
-      <c r="C108" t="n" s="68">
+      <c r="C108" t="n" s="80">
         <v>32.0</v>
       </c>
       <c r="D108" t="n">
@@ -15098,7 +15202,7 @@
       <c r="B109" t="s">
         <v>40</v>
       </c>
-      <c r="C109" t="n" s="68">
+      <c r="C109" t="n" s="80">
         <v>78.0</v>
       </c>
       <c r="D109" t="n">
@@ -15170,7 +15274,7 @@
       <c r="Z109" t="n">
         <v>133.0</v>
       </c>
-      <c r="AA109" t="n" s="68">
+      <c r="AA109" t="n" s="80">
         <v>24.0</v>
       </c>
       <c r="AB109" t="n">
@@ -15254,10 +15358,10 @@
       <c r="K110" t="n">
         <v>0.0</v>
       </c>
-      <c r="L110" t="n" s="68">
+      <c r="L110" t="n" s="80">
         <v>6.9</v>
       </c>
-      <c r="M110" t="n" s="68">
+      <c r="M110" t="n" s="80">
         <v>3.9</v>
       </c>
       <c r="N110" t="n">
@@ -15299,7 +15403,7 @@
       <c r="Z110" t="n">
         <v>155.0</v>
       </c>
-      <c r="AA110" t="n" s="68">
+      <c r="AA110" t="n" s="80">
         <v>27.0</v>
       </c>
       <c r="AB110" t="n">
@@ -15428,11 +15532,11 @@
       <c r="Z111" t="n">
         <v>192.0</v>
       </c>
-      <c r="AA111" t="n" s="68">
+      <c r="AA111" t="n" s="80">
         <v>26.0</v>
       </c>
       <c r="AB111" s="8"/>
-      <c r="AC111" t="n" s="48">
+      <c r="AC111" t="n" s="56">
         <v>3.0</v>
       </c>
       <c r="AD111" t="n">
@@ -15450,7 +15554,7 @@
       <c r="AH111" t="n">
         <v>0.0</v>
       </c>
-      <c r="AI111" t="n" s="28">
+      <c r="AI111" t="n" s="32">
         <v>1.0</v>
       </c>
       <c r="AJ111" t="n">
@@ -15488,7 +15592,7 @@
       <c r="C112" t="n">
         <v>72.0</v>
       </c>
-      <c r="D112" t="n" s="68">
+      <c r="D112" t="n" s="80">
         <v>126.0</v>
       </c>
       <c r="E112" t="s">
@@ -15616,7 +15720,7 @@
       <c r="B113" t="s">
         <v>40</v>
       </c>
-      <c r="C113" t="n" s="68">
+      <c r="C113" t="n" s="80">
         <v>22.0</v>
       </c>
       <c r="D113" t="n">
@@ -16263,7 +16367,7 @@
       <c r="B118" t="s">
         <v>40</v>
       </c>
-      <c r="C118" t="n" s="68">
+      <c r="C118" t="n" s="80">
         <v>24.0</v>
       </c>
       <c r="D118" t="n">
@@ -16422,7 +16526,7 @@
       <c r="L119" t="n">
         <v>4.1</v>
       </c>
-      <c r="M119" t="n" s="68">
+      <c r="M119" t="n" s="80">
         <v>4.3</v>
       </c>
       <c r="N119" t="n">
@@ -16523,7 +16627,7 @@
       <c r="B120" t="s">
         <v>40</v>
       </c>
-      <c r="C120" t="n" s="68">
+      <c r="C120" t="n" s="80">
         <v>25.0</v>
       </c>
       <c r="D120" t="n">
@@ -17087,7 +17191,7 @@
       <c r="R124" t="n">
         <v>1.0</v>
       </c>
-      <c r="S124" t="n" s="68">
+      <c r="S124" t="n" s="80">
         <v>24.0</v>
       </c>
       <c r="T124" t="n">
@@ -17198,7 +17302,7 @@
       <c r="L125" t="n">
         <v>2.3</v>
       </c>
-      <c r="M125" t="n" s="68">
+      <c r="M125" t="n" s="80">
         <v>3.9</v>
       </c>
       <c r="N125" t="n">
@@ -17237,7 +17341,7 @@
       <c r="Y125" t="n">
         <v>1.0</v>
       </c>
-      <c r="Z125" t="n" s="68">
+      <c r="Z125" t="n" s="80">
         <v>526.0</v>
       </c>
       <c r="AA125" t="n">

</xml_diff>

<commit_message>
Main and File with child were fixed. library started
</commit_message>
<xml_diff>
--- a/data_CABG_PCI_2_coloring.xlsx
+++ b/data_CABG_PCI_2_coloring.xlsx
@@ -443,7 +443,7 @@
     <t>08.05.2009</t>
   </si>
   <si>
-    <t>13.05.2009</t>
+    <t>13,05,2009</t>
   </si>
   <si>
     <t>12.05.2009</t>
@@ -6709,7 +6709,7 @@
       <c r="O41" t="n">
         <v>38.0</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" t="s" s="80">
         <v>133</v>
       </c>
       <c r="Q41" t="n">
@@ -8908,7 +8908,7 @@
       <c r="O58" t="n">
         <v>76.0</v>
       </c>
-      <c r="P58" t="s" s="80">
+      <c r="P58" t="s" s="32">
         <v>123</v>
       </c>
       <c r="Q58" t="n">
@@ -11740,7 +11740,7 @@
       <c r="O80" t="n">
         <v>85.0</v>
       </c>
-      <c r="P80" t="s" s="80">
+      <c r="P80" t="s" s="32">
         <v>137</v>
       </c>
       <c r="Q80" t="n">

</xml_diff>